<commit_message>
schedule now produces a simple excel document with a list of people
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -15,15 +15,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>world!</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Bin Filler</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Karen</t>
+  </si>
+  <si>
+    <t>Lohse</t>
+  </si>
+  <si>
+    <t>Forklift</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> George</t>
+  </si>
+  <si>
+    <t>Dunn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Don</t>
+  </si>
+  <si>
+    <t>Coles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> George C</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Line Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parveen</t>
+  </si>
+  <si>
+    <t>Gopal</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isabel</t>
+  </si>
+  <si>
+    <t>Roseen</t>
+  </si>
+  <si>
+    <t>Sorter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jean</t>
+  </si>
+  <si>
+    <t>Strachan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wendy</t>
+  </si>
+  <si>
+    <t>Casorso</t>
+  </si>
+  <si>
+    <t>Non Rotational</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elaine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Janeanne</t>
+  </si>
+  <si>
+    <t>Reiswig</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sandra</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Joyce</t>
+  </si>
+  <si>
+    <t>Salga</t>
   </si>
 </sst>
 </file>
@@ -362,7 +458,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -370,20 +466,228 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shift now shows up in english
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
   <si>
     <t>Position</t>
   </si>
@@ -35,6 +35,18 @@
     <t>Station</t>
   </si>
   <si>
+    <t>BMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dale </t>
+  </si>
+  <si>
+    <t>Driscoll</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
     <t>Bin Filler</t>
   </si>
   <si>
@@ -74,6 +86,12 @@
     <t>Gopal</t>
   </si>
   <si>
+    <t xml:space="preserve"> Lori</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
     <t>QC</t>
   </si>
   <si>
@@ -83,7 +101,94 @@
     <t>Roseen</t>
   </si>
   <si>
-    <t>Sorter</t>
+    <t xml:space="preserve"> Wendy</t>
+  </si>
+  <si>
+    <t>Casorso</t>
+  </si>
+  <si>
+    <t>Palletizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Javed</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Stamping</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jane</t>
+  </si>
+  <si>
+    <t>Wu</t>
+  </si>
+  <si>
+    <t>Non Rotational</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elaine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Janeanne</t>
+  </si>
+  <si>
+    <t>Reiswig</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sandra</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>A Bliss</t>
+  </si>
+  <si>
+    <t>Pauline</t>
+  </si>
+  <si>
+    <t>Palatin</t>
+  </si>
+  <si>
+    <t>B Bliss</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cheryl</t>
+  </si>
+  <si>
+    <t>Deboer</t>
+  </si>
+  <si>
+    <t>F/L Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Margie</t>
+  </si>
+  <si>
+    <t>Butcher</t>
+  </si>
+  <si>
+    <t>F/L Dumper (6:45am)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juanita</t>
+  </si>
+  <si>
+    <t>Windels</t>
+  </si>
+  <si>
+    <t>F/L Paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Branden</t>
+  </si>
+  <si>
+    <t>Dubrett</t>
+  </si>
+  <si>
+    <t>Sort - A1</t>
   </si>
   <si>
     <t xml:space="preserve"> Jean</t>
@@ -92,34 +197,202 @@
     <t>Strachan</t>
   </si>
   <si>
-    <t xml:space="preserve"> Wendy</t>
-  </si>
-  <si>
-    <t>Casorso</t>
-  </si>
-  <si>
-    <t>Non Rotational</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elaine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Janeanne</t>
-  </si>
-  <si>
-    <t>Reiswig</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sandra</t>
-  </si>
-  <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Joyce</t>
-  </si>
-  <si>
-    <t>Salga</t>
+    <t>Sort - A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Janice</t>
+  </si>
+  <si>
+    <t>Koyama</t>
+  </si>
+  <si>
+    <t>Sort - A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul</t>
+  </si>
+  <si>
+    <t>Jansen</t>
+  </si>
+  <si>
+    <t>Sort - A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ed</t>
+  </si>
+  <si>
+    <t>Fehr</t>
+  </si>
+  <si>
+    <t>Sort - A5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gerald</t>
+  </si>
+  <si>
+    <t>Kunz</t>
+  </si>
+  <si>
+    <t>Sort - A6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ron</t>
+  </si>
+  <si>
+    <t>Engene</t>
+  </si>
+  <si>
+    <t>Sort - A7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jerry</t>
+  </si>
+  <si>
+    <t>Sort - A8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurdev</t>
+  </si>
+  <si>
+    <t>Bains</t>
+  </si>
+  <si>
+    <t>Flow Control - A8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shannon</t>
+  </si>
+  <si>
+    <t>Flow Control - A9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fay</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Flow Control - A10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dora</t>
+  </si>
+  <si>
+    <t>Flow Control - A11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ann</t>
+  </si>
+  <si>
+    <t>Cloutier</t>
+  </si>
+  <si>
+    <t>Fill - A12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gail</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Fill - A13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nadine</t>
+  </si>
+  <si>
+    <t>Boltz</t>
+  </si>
+  <si>
+    <t>Fill - A14</t>
+  </si>
+  <si>
+    <t>Donnely</t>
+  </si>
+  <si>
+    <t>Fill - A15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ross</t>
+  </si>
+  <si>
+    <t>Izod</t>
+  </si>
+  <si>
+    <t>Fill - B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Judy</t>
+  </si>
+  <si>
+    <t>Skrove</t>
+  </si>
+  <si>
+    <t>Fill - B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Doris</t>
+  </si>
+  <si>
+    <t>Reynolds</t>
+  </si>
+  <si>
+    <t>Fill - B3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tim</t>
+  </si>
+  <si>
+    <t>Fill - B4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rick</t>
+  </si>
+  <si>
+    <t>Sehn</t>
+  </si>
+  <si>
+    <t>Sort - B5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kathy</t>
+  </si>
+  <si>
+    <t>Yates</t>
+  </si>
+  <si>
+    <t>Sort - B6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barb</t>
+  </si>
+  <si>
+    <t>Silvester</t>
+  </si>
+  <si>
+    <t>Sort - B7</t>
+  </si>
+  <si>
+    <t>Matsalla</t>
+  </si>
+  <si>
+    <t>Sort - B8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Debbie</t>
+  </si>
+  <si>
+    <t>Szing</t>
+  </si>
+  <si>
+    <t>Sort - B9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marcella</t>
+  </si>
+  <si>
+    <t>Bartolomeoli</t>
   </si>
 </sst>
 </file>
@@ -458,7 +731,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,6 +769,9 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
@@ -505,13 +781,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -522,13 +801,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -539,13 +821,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -556,13 +841,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
@@ -573,13 +861,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -590,7 +881,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -598,6 +889,9 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
@@ -607,13 +901,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -624,13 +921,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -641,13 +941,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -658,13 +961,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
@@ -675,18 +981,661 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
+      <c r="D13" t="s">
+        <v>9</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
       </c>
       <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added some comments on describing how the create_schedule agorith works
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
   <si>
     <t>Position</t>
   </si>
@@ -77,6 +77,24 @@
     <t>Brown</t>
   </si>
   <si>
+    <t xml:space="preserve"> Ron</t>
+  </si>
+  <si>
+    <t>Engene</t>
+  </si>
+  <si>
+    <t>Afternoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jerry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fay</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
     <t>Line Operator</t>
   </si>
   <si>
@@ -92,6 +110,12 @@
     <t>Carter</t>
   </si>
   <si>
+    <t xml:space="preserve"> Linda</t>
+  </si>
+  <si>
+    <t>St. Amand</t>
+  </si>
+  <si>
     <t>QC</t>
   </si>
   <si>
@@ -107,6 +131,12 @@
     <t>Casorso</t>
   </si>
   <si>
+    <t xml:space="preserve"> Shannon</t>
+  </si>
+  <si>
+    <t>Fehr</t>
+  </si>
+  <si>
     <t>Palletizer</t>
   </si>
   <si>
@@ -143,6 +173,12 @@
     <t>Martin</t>
   </si>
   <si>
+    <t xml:space="preserve"> Joyce</t>
+  </si>
+  <si>
+    <t>Salga</t>
+  </si>
+  <si>
     <t>A Bliss</t>
   </si>
   <si>
@@ -221,9 +257,6 @@
     <t xml:space="preserve"> Ed</t>
   </si>
   <si>
-    <t>Fehr</t>
-  </si>
-  <si>
     <t>Sort - A5</t>
   </si>
   <si>
@@ -236,163 +269,169 @@
     <t>Sort - A6</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ron</t>
-  </si>
-  <si>
-    <t>Engene</t>
+    <t xml:space="preserve"> Gurdev</t>
+  </si>
+  <si>
+    <t>Bains</t>
   </si>
   <si>
     <t>Sort - A7</t>
   </si>
   <si>
-    <t xml:space="preserve"> Jerry</t>
+    <t xml:space="preserve"> Dora</t>
   </si>
   <si>
     <t>Sort - A8</t>
   </si>
   <si>
-    <t xml:space="preserve"> Gurdev</t>
-  </si>
-  <si>
-    <t>Bains</t>
+    <t xml:space="preserve"> Ann</t>
+  </si>
+  <si>
+    <t>Cloutier</t>
   </si>
   <si>
     <t>Flow Control - A8</t>
   </si>
   <si>
-    <t xml:space="preserve"> Shannon</t>
+    <t xml:space="preserve"> Gail</t>
+  </si>
+  <si>
+    <t>Johnson</t>
   </si>
   <si>
     <t>Flow Control - A9</t>
   </si>
   <si>
-    <t xml:space="preserve"> Fay</t>
-  </si>
-  <si>
-    <t>Lee</t>
+    <t xml:space="preserve"> Nadine</t>
+  </si>
+  <si>
+    <t>Boltz</t>
   </si>
   <si>
     <t>Flow Control - A10</t>
   </si>
   <si>
-    <t xml:space="preserve"> Dora</t>
+    <t>Donnely</t>
   </si>
   <si>
     <t>Flow Control - A11</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ann</t>
-  </si>
-  <si>
-    <t>Cloutier</t>
+    <t xml:space="preserve"> Ross</t>
+  </si>
+  <si>
+    <t>Izod</t>
   </si>
   <si>
     <t>Fill - A12</t>
   </si>
   <si>
-    <t xml:space="preserve"> Gail</t>
-  </si>
-  <si>
-    <t>Johnson</t>
+    <t xml:space="preserve"> Judy</t>
+  </si>
+  <si>
+    <t>Skrove</t>
   </si>
   <si>
     <t>Fill - A13</t>
   </si>
   <si>
-    <t xml:space="preserve"> Nadine</t>
-  </si>
-  <si>
-    <t>Boltz</t>
+    <t xml:space="preserve"> Doris</t>
+  </si>
+  <si>
+    <t>Reynolds</t>
   </si>
   <si>
     <t>Fill - A14</t>
   </si>
   <si>
-    <t>Donnely</t>
+    <t xml:space="preserve"> Tim</t>
   </si>
   <si>
     <t>Fill - A15</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ross</t>
-  </si>
-  <si>
-    <t>Izod</t>
+    <t xml:space="preserve"> Rick</t>
+  </si>
+  <si>
+    <t>Sehn</t>
   </si>
   <si>
     <t>Fill - B1</t>
   </si>
   <si>
-    <t xml:space="preserve"> Judy</t>
-  </si>
-  <si>
-    <t>Skrove</t>
+    <t xml:space="preserve"> Kathy</t>
+  </si>
+  <si>
+    <t>Yates</t>
   </si>
   <si>
     <t>Fill - B2</t>
   </si>
   <si>
-    <t xml:space="preserve"> Doris</t>
-  </si>
-  <si>
-    <t>Reynolds</t>
+    <t xml:space="preserve"> Barb</t>
+  </si>
+  <si>
+    <t>Silvester</t>
   </si>
   <si>
     <t>Fill - B3</t>
   </si>
   <si>
-    <t xml:space="preserve"> Tim</t>
+    <t>Matsalla</t>
   </si>
   <si>
     <t>Fill - B4</t>
   </si>
   <si>
-    <t xml:space="preserve"> Rick</t>
-  </si>
-  <si>
-    <t>Sehn</t>
+    <t xml:space="preserve"> Debbie</t>
+  </si>
+  <si>
+    <t>Szing</t>
   </si>
   <si>
     <t>Sort - B5</t>
   </si>
   <si>
-    <t xml:space="preserve"> Kathy</t>
-  </si>
-  <si>
-    <t>Yates</t>
+    <t xml:space="preserve"> Marcella</t>
+  </si>
+  <si>
+    <t>Bartolomeoli</t>
   </si>
   <si>
     <t>Sort - B6</t>
   </si>
   <si>
-    <t xml:space="preserve"> Barb</t>
-  </si>
-  <si>
-    <t>Silvester</t>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Young</t>
   </si>
   <si>
     <t>Sort - B7</t>
   </si>
   <si>
-    <t>Matsalla</t>
+    <t xml:space="preserve"> Jennifer </t>
+  </si>
+  <si>
+    <t>Knight</t>
   </si>
   <si>
     <t>Sort - B8</t>
   </si>
   <si>
-    <t xml:space="preserve"> Debbie</t>
-  </si>
-  <si>
-    <t>Szing</t>
+    <t xml:space="preserve"> Cindy</t>
+  </si>
+  <si>
+    <t>Stubbs</t>
   </si>
   <si>
     <t>Sort - B9</t>
   </si>
   <si>
-    <t xml:space="preserve"> Marcella</t>
-  </si>
-  <si>
-    <t>Bartolomeoli</t>
+    <t xml:space="preserve"> Judy Ann</t>
+  </si>
+  <si>
+    <t>Seymour</t>
   </si>
 </sst>
 </file>
@@ -731,7 +770,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -861,16 +900,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -881,16 +920,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -901,16 +940,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -921,13 +960,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -941,13 +980,13 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -961,16 +1000,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
@@ -981,13 +1020,13 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -1001,13 +1040,13 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -1021,16 +1060,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
         <v>4</v>
@@ -1041,13 +1080,13 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -1061,13 +1100,13 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
         <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -1081,13 +1120,13 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -1101,13 +1140,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -1121,16 +1160,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
@@ -1141,16 +1180,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -1161,13 +1200,13 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -1181,13 +1220,13 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
@@ -1201,13 +1240,13 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
@@ -1221,13 +1260,13 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1241,13 +1280,13 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
@@ -1261,13 +1300,13 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -1281,13 +1320,13 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -1301,13 +1340,13 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -1321,13 +1360,13 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
@@ -1341,13 +1380,13 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
@@ -1361,13 +1400,13 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -1381,13 +1420,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -1401,13 +1440,13 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D34" t="s">
         <v>9</v>
@@ -1421,13 +1460,13 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
@@ -1441,13 +1480,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D36" t="s">
         <v>9</v>
@@ -1461,13 +1500,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
@@ -1481,13 +1520,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
@@ -1501,13 +1540,13 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
@@ -1521,13 +1560,13 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
@@ -1541,13 +1580,13 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -1561,13 +1600,13 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
@@ -1581,13 +1620,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
@@ -1601,13 +1640,13 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
@@ -1621,21 +1660,141 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" t="s">
         <v>123</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
         <v>124</v>
       </c>
-      <c r="C45" t="s">
+      <c r="B47" t="s">
         <v>125</v>
       </c>
-      <c r="D45" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="C47" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
schedule bug fixes with the PP_NS
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>Position</t>
   </si>
@@ -38,10 +38,10 @@
     <t>Bin Filler</t>
   </si>
   <si>
-    <t xml:space="preserve"> Karen</t>
-  </si>
-  <si>
-    <t>Lohse</t>
+    <t xml:space="preserve"> Doris</t>
+  </si>
+  <si>
+    <t>Reynolds</t>
   </si>
   <si>
     <t>Day</t>
@@ -53,6 +53,27 @@
     <t>Winfield</t>
   </si>
   <si>
+    <t xml:space="preserve"> Zabada</t>
+  </si>
+  <si>
+    <t>Mohammed</t>
+  </si>
+  <si>
+    <t>Afternoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sukhwinder</t>
+  </si>
+  <si>
+    <t>Gakhal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kuldip</t>
+  </si>
+  <si>
+    <t>Buttar</t>
+  </si>
+  <si>
     <t>Forklift</t>
   </si>
   <si>
@@ -74,6 +95,21 @@
     <t>Brown</t>
   </si>
   <si>
+    <t xml:space="preserve"> Ron</t>
+  </si>
+  <si>
+    <t>Engene</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jerry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fay</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
     <t>Line Operator</t>
   </si>
   <si>
@@ -83,6 +119,12 @@
     <t>Gopal</t>
   </si>
   <si>
+    <t xml:space="preserve"> Lori</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
     <t>QC</t>
   </si>
   <si>
@@ -92,6 +134,12 @@
     <t>Roseen</t>
   </si>
   <si>
+    <t xml:space="preserve"> Wendy</t>
+  </si>
+  <si>
+    <t>Casorso</t>
+  </si>
+  <si>
     <t>Non Rotational</t>
   </si>
   <si>
@@ -108,6 +156,18 @@
   </si>
   <si>
     <t>Martin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brian</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Joyce</t>
+  </si>
+  <si>
+    <t>Salga</t>
   </si>
 </sst>
 </file>
@@ -446,7 +506,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,16 +556,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -516,7 +576,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -525,7 +585,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -536,7 +596,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -576,13 +636,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -596,13 +656,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -616,16 +676,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -636,21 +696,221 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed isSortersFull, bug was causing it to add up the sorters incorrectly.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="164">
   <si>
     <t>Position</t>
   </si>
@@ -125,6 +125,21 @@
     <t>Carter</t>
   </si>
   <si>
+    <t>A Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Linda</t>
+  </si>
+  <si>
+    <t>St. Amand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Julie</t>
+  </si>
+  <si>
+    <t>Hackman</t>
+  </si>
+  <si>
     <t>QC</t>
   </si>
   <si>
@@ -140,6 +155,66 @@
     <t>Casorso</t>
   </si>
   <si>
+    <t xml:space="preserve"> Shannon</t>
+  </si>
+  <si>
+    <t>Fehr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ann</t>
+  </si>
+  <si>
+    <t>Cloutier</t>
+  </si>
+  <si>
+    <t>Palletizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Javed</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Labeller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gail</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tirath</t>
+  </si>
+  <si>
+    <t>Mann</t>
+  </si>
+  <si>
+    <t>Trays</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ranjeet</t>
+  </si>
+  <si>
+    <t>Deol</t>
+  </si>
+  <si>
+    <t>Stamping</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jane</t>
+  </si>
+  <si>
+    <t>Wu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurdev </t>
+  </si>
+  <si>
+    <t>Kajla</t>
+  </si>
+  <si>
     <t>Non Rotational</t>
   </si>
   <si>
@@ -168,6 +243,270 @@
   </si>
   <si>
     <t>Salga</t>
+  </si>
+  <si>
+    <t>A Bliss</t>
+  </si>
+  <si>
+    <t>Pauline</t>
+  </si>
+  <si>
+    <t>Palatin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cheryl</t>
+  </si>
+  <si>
+    <t>Deboer</t>
+  </si>
+  <si>
+    <t>F/L Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juanita</t>
+  </si>
+  <si>
+    <t>Windels</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Branden</t>
+  </si>
+  <si>
+    <t>Dubrett</t>
+  </si>
+  <si>
+    <t>F/L Dumper (6:45am)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Margie</t>
+  </si>
+  <si>
+    <t>Butcher</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chris</t>
+  </si>
+  <si>
+    <t>Bauer</t>
+  </si>
+  <si>
+    <t>Sort - A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jean</t>
+  </si>
+  <si>
+    <t>Strachan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurdev</t>
+  </si>
+  <si>
+    <t>Bains</t>
+  </si>
+  <si>
+    <t>Sort - A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Janice</t>
+  </si>
+  <si>
+    <t>Koyama</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Judy</t>
+  </si>
+  <si>
+    <t>Matsalla</t>
+  </si>
+  <si>
+    <t>Sort - A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul</t>
+  </si>
+  <si>
+    <t>Jansen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Debbie</t>
+  </si>
+  <si>
+    <t>Szing</t>
+  </si>
+  <si>
+    <t>Sort - A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Judy Ann</t>
+  </si>
+  <si>
+    <t>Seymour</t>
+  </si>
+  <si>
+    <t>Sort - A5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gerald</t>
+  </si>
+  <si>
+    <t>Kunz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sue</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>Sort - A6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dora</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lindi</t>
+  </si>
+  <si>
+    <t>Karmason</t>
+  </si>
+  <si>
+    <t>Sort - A7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nadine</t>
+  </si>
+  <si>
+    <t>Boltz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bobby </t>
+  </si>
+  <si>
+    <t>Kovacs</t>
+  </si>
+  <si>
+    <t>Sort - A8</t>
+  </si>
+  <si>
+    <t>Donnely</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Catherine</t>
+  </si>
+  <si>
+    <t>Knox</t>
+  </si>
+  <si>
+    <t>Flow Control - A8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ross</t>
+  </si>
+  <si>
+    <t>Izod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rukhmani</t>
+  </si>
+  <si>
+    <t>Reddy</t>
+  </si>
+  <si>
+    <t>Flow Control - A9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dale </t>
+  </si>
+  <si>
+    <t>Driscoll</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vickee</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Flow Control - A10</t>
+  </si>
+  <si>
+    <t>Skrove</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mary-Ann</t>
+  </si>
+  <si>
+    <t>Korthals</t>
+  </si>
+  <si>
+    <t>Flow Control - A11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tim</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sylvia</t>
+  </si>
+  <si>
+    <t>Friedrich</t>
+  </si>
+  <si>
+    <t>Fill - A12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Karen</t>
+  </si>
+  <si>
+    <t>Lohse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barb</t>
+  </si>
+  <si>
+    <t>Tyrrell</t>
+  </si>
+  <si>
+    <t>Fill - A13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rick</t>
+  </si>
+  <si>
+    <t>Sehn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ramji</t>
+  </si>
+  <si>
+    <t>Badhan</t>
+  </si>
+  <si>
+    <t>Fill - A14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kathy</t>
+  </si>
+  <si>
+    <t>Yates</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurpal </t>
+  </si>
+  <si>
+    <t>Nijjar</t>
+  </si>
+  <si>
+    <t>Fill - A15</t>
+  </si>
+  <si>
+    <t>Silvester</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sohan</t>
   </si>
 </sst>
 </file>
@@ -506,7 +845,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -765,10 +1104,10 @@
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -776,7 +1115,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -785,7 +1124,7 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -796,7 +1135,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
@@ -808,7 +1147,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
         <v>11</v>
@@ -822,7 +1161,7 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -839,16 +1178,16 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -859,10 +1198,10 @@
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -879,16 +1218,16 @@
         <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F19" t="s">
         <v>11</v>
@@ -896,21 +1235,981 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
         <v>10</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>36</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>36</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>36</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s">
+        <v>36</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" t="s">
+        <v>121</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>36</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" t="s">
+        <v>125</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s">
+        <v>36</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" t="s">
+        <v>127</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" t="s">
+        <v>36</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" t="s">
+        <v>130</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s">
+        <v>36</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>128</v>
+      </c>
+      <c r="B54" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" t="s">
+        <v>132</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" t="s">
+        <v>36</v>
+      </c>
+      <c r="F54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" t="s">
+        <v>36</v>
+      </c>
+      <c r="F55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" t="s">
+        <v>36</v>
+      </c>
+      <c r="F56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" t="s">
+        <v>139</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>36</v>
+      </c>
+      <c r="F57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" t="s">
+        <v>141</v>
+      </c>
+      <c r="D58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" t="s">
+        <v>36</v>
+      </c>
+      <c r="F58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>36</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>142</v>
+      </c>
+      <c r="B60" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" t="s">
+        <v>145</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" t="s">
+        <v>36</v>
+      </c>
+      <c r="F60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>146</v>
+      </c>
+      <c r="B61" t="s">
+        <v>147</v>
+      </c>
+      <c r="C61" t="s">
+        <v>148</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" t="s">
+        <v>149</v>
+      </c>
+      <c r="C62" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62" t="s">
+        <v>36</v>
+      </c>
+      <c r="F62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>151</v>
+      </c>
+      <c r="B63" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" t="s">
+        <v>153</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>36</v>
+      </c>
+      <c r="F63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>151</v>
+      </c>
+      <c r="B64" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" t="s">
+        <v>155</v>
+      </c>
+      <c r="D64" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>156</v>
+      </c>
+      <c r="B65" t="s">
+        <v>157</v>
+      </c>
+      <c r="C65" t="s">
+        <v>158</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>36</v>
+      </c>
+      <c r="F65" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>156</v>
+      </c>
+      <c r="B66" t="s">
+        <v>159</v>
+      </c>
+      <c r="C66" t="s">
+        <v>160</v>
+      </c>
+      <c r="D66" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66" t="s">
+        <v>36</v>
+      </c>
+      <c r="F66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>161</v>
+      </c>
+      <c r="B67" t="s">
+        <v>149</v>
+      </c>
+      <c r="C67" t="s">
+        <v>162</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>36</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>161</v>
+      </c>
+      <c r="B68" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" t="s">
+        <v>65</v>
+      </c>
+      <c r="D68" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" t="s">
+        <v>36</v>
+      </c>
+      <c r="F68" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
unfilled position returns correct positions
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
   <si>
     <t>Position</t>
   </si>
@@ -35,46 +35,154 @@
     <t>Station</t>
   </si>
   <si>
-    <t>Bin Filler</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Doris</t>
-  </si>
-  <si>
-    <t>Reynolds</t>
+    <t>Line Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parveen</t>
+  </si>
+  <si>
+    <t>Gopal</t>
   </si>
   <si>
     <t>Day</t>
   </si>
   <si>
-    <t>Presize</t>
+    <t>A Line</t>
   </si>
   <si>
     <t>Winfield</t>
   </si>
   <si>
-    <t xml:space="preserve"> Zabada</t>
-  </si>
-  <si>
-    <t>Mohammed</t>
+    <t xml:space="preserve"> Lori</t>
+  </si>
+  <si>
+    <t>Carter</t>
   </si>
   <si>
     <t>Afternoon</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sukhwinder</t>
-  </si>
-  <si>
-    <t>Gakhal</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kuldip</t>
-  </si>
-  <si>
-    <t>Buttar</t>
-  </si>
-  <si>
-    <t>Forklift</t>
+    <t>QC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isabel</t>
+  </si>
+  <si>
+    <t>Roseen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wendy</t>
+  </si>
+  <si>
+    <t>Casorso</t>
+  </si>
+  <si>
+    <t>Palletizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Javed</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Labeller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gail</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tirath</t>
+  </si>
+  <si>
+    <t>Mann</t>
+  </si>
+  <si>
+    <t>Trays</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ranjeet</t>
+  </si>
+  <si>
+    <t>Deol</t>
+  </si>
+  <si>
+    <t>Stamping</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jane</t>
+  </si>
+  <si>
+    <t>Wu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurdev </t>
+  </si>
+  <si>
+    <t>Kajla</t>
+  </si>
+  <si>
+    <t>A Bliss</t>
+  </si>
+  <si>
+    <t>Pauline</t>
+  </si>
+  <si>
+    <t>Palatin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cheryl</t>
+  </si>
+  <si>
+    <t>Deboer</t>
+  </si>
+  <si>
+    <t>F/L Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juanita</t>
+  </si>
+  <si>
+    <t>Windels</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Branden</t>
+  </si>
+  <si>
+    <t>Dubrett</t>
+  </si>
+  <si>
+    <t>F/L Dumper (6:45am)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Margie</t>
+  </si>
+  <si>
+    <t>Butcher</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chris</t>
+  </si>
+  <si>
+    <t>Bauer</t>
+  </si>
+  <si>
+    <t>Sort - A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elaine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurdev</t>
+  </si>
+  <si>
+    <t>Bains</t>
+  </si>
+  <si>
+    <t>Sort - A2</t>
   </si>
   <si>
     <t xml:space="preserve"> George</t>
@@ -83,55 +191,178 @@
     <t>Dunn</t>
   </si>
   <si>
+    <t xml:space="preserve"> Ross</t>
+  </si>
+  <si>
+    <t>Izod</t>
+  </si>
+  <si>
+    <t>Sort - A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jean</t>
+  </si>
+  <si>
+    <t>Strachan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Karen</t>
+  </si>
+  <si>
+    <t>Lohse</t>
+  </si>
+  <si>
+    <t>Sort - A4</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Don</t>
   </si>
   <si>
     <t>Coles</t>
   </si>
   <si>
+    <t xml:space="preserve"> Kathy</t>
+  </si>
+  <si>
+    <t>Yates</t>
+  </si>
+  <si>
+    <t>Sort - A5</t>
+  </si>
+  <si>
+    <t>UNFILLED POSITION</t>
+  </si>
+  <si>
     <t xml:space="preserve"> George C</t>
   </si>
   <si>
     <t>Brown</t>
   </si>
   <si>
+    <t xml:space="preserve"> Barb</t>
+  </si>
+  <si>
+    <t>Silvester</t>
+  </si>
+  <si>
+    <t>Sort - A6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Janice</t>
+  </si>
+  <si>
+    <t>Koyama</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Judy</t>
+  </si>
+  <si>
+    <t>Matsalla</t>
+  </si>
+  <si>
+    <t>Sort - A7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul</t>
+  </si>
+  <si>
+    <t>Jansen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Debbie</t>
+  </si>
+  <si>
+    <t>Szing</t>
+  </si>
+  <si>
+    <t>Sort - A8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ed</t>
+  </si>
+  <si>
+    <t>Fehr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Linda</t>
+  </si>
+  <si>
+    <t>St. Amand</t>
+  </si>
+  <si>
+    <t>Flow Control - A8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gerald</t>
+  </si>
+  <si>
+    <t>Kunz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sandra</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Flow Control - A9</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Ron</t>
   </si>
   <si>
     <t>Engene</t>
   </si>
   <si>
+    <t xml:space="preserve"> Judy Ann</t>
+  </si>
+  <si>
+    <t>Seymour</t>
+  </si>
+  <si>
+    <t>Flow Control - A10</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Jerry</t>
   </si>
   <si>
+    <t xml:space="preserve"> Sue</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>Flow Control - A11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shannon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lindi</t>
+  </si>
+  <si>
+    <t>Karmason</t>
+  </si>
+  <si>
+    <t>Fill - A12</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Fay</t>
   </si>
   <si>
     <t>Lee</t>
   </si>
   <si>
-    <t>Line Operator</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Parveen</t>
-  </si>
-  <si>
-    <t>Gopal</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lori</t>
-  </si>
-  <si>
-    <t>Carter</t>
-  </si>
-  <si>
-    <t>A Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Linda</t>
-  </si>
-  <si>
-    <t>St. Amand</t>
+    <t xml:space="preserve"> Bobby </t>
+  </si>
+  <si>
+    <t>Kovacs</t>
+  </si>
+  <si>
+    <t>Fill - A13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dora</t>
   </si>
   <si>
     <t xml:space="preserve"> Julie</t>
@@ -140,25 +371,7 @@
     <t>Hackman</t>
   </si>
   <si>
-    <t>QC</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Isabel</t>
-  </si>
-  <si>
-    <t>Roseen</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wendy</t>
-  </si>
-  <si>
-    <t>Casorso</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Shannon</t>
-  </si>
-  <si>
-    <t>Fehr</t>
+    <t>Fill - A14</t>
   </si>
   <si>
     <t xml:space="preserve"> Ann</t>
@@ -167,214 +380,13 @@
     <t>Cloutier</t>
   </si>
   <si>
-    <t>Palletizer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Javed</t>
-  </si>
-  <si>
-    <t>Ali</t>
-  </si>
-  <si>
-    <t>Labeller</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gail</t>
-  </si>
-  <si>
-    <t>Johnson</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tirath</t>
-  </si>
-  <si>
-    <t>Mann</t>
-  </si>
-  <si>
-    <t>Trays</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ranjeet</t>
-  </si>
-  <si>
-    <t>Deol</t>
-  </si>
-  <si>
-    <t>Stamping</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jane</t>
-  </si>
-  <si>
-    <t>Wu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gurdev </t>
-  </si>
-  <si>
-    <t>Kajla</t>
-  </si>
-  <si>
-    <t>Non Rotational</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elaine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Janeanne</t>
-  </si>
-  <si>
-    <t>Reiswig</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sandra</t>
-  </si>
-  <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Brian</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Joyce</t>
-  </si>
-  <si>
-    <t>Salga</t>
-  </si>
-  <si>
-    <t>A Bliss</t>
-  </si>
-  <si>
-    <t>Pauline</t>
-  </si>
-  <si>
-    <t>Palatin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cheryl</t>
-  </si>
-  <si>
-    <t>Deboer</t>
-  </si>
-  <si>
-    <t>F/L Operator</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Juanita</t>
-  </si>
-  <si>
-    <t>Windels</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Branden</t>
-  </si>
-  <si>
-    <t>Dubrett</t>
-  </si>
-  <si>
-    <t>F/L Dumper (6:45am)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Margie</t>
-  </si>
-  <si>
-    <t>Butcher</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chris</t>
-  </si>
-  <si>
-    <t>Bauer</t>
-  </si>
-  <si>
-    <t>Sort - A1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jean</t>
-  </si>
-  <si>
-    <t>Strachan</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gurdev</t>
-  </si>
-  <si>
-    <t>Bains</t>
-  </si>
-  <si>
-    <t>Sort - A2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Janice</t>
-  </si>
-  <si>
-    <t>Koyama</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Judy</t>
-  </si>
-  <si>
-    <t>Matsalla</t>
-  </si>
-  <si>
-    <t>Sort - A3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paul</t>
-  </si>
-  <si>
-    <t>Jansen</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Debbie</t>
-  </si>
-  <si>
-    <t>Szing</t>
-  </si>
-  <si>
-    <t>Sort - A4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ed</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Judy Ann</t>
-  </si>
-  <si>
-    <t>Seymour</t>
-  </si>
-  <si>
-    <t>Sort - A5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gerald</t>
-  </si>
-  <si>
-    <t>Kunz</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sue</t>
-  </si>
-  <si>
-    <t>Marks</t>
-  </si>
-  <si>
-    <t>Sort - A6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dora</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lindi</t>
-  </si>
-  <si>
-    <t>Karmason</t>
-  </si>
-  <si>
-    <t>Sort - A7</t>
+    <t xml:space="preserve"> Catherine</t>
+  </si>
+  <si>
+    <t>Knox</t>
+  </si>
+  <si>
+    <t>Fill - A15</t>
   </si>
   <si>
     <t xml:space="preserve"> Nadine</t>
@@ -383,130 +395,10 @@
     <t>Boltz</t>
   </si>
   <si>
-    <t xml:space="preserve"> Bobby </t>
-  </si>
-  <si>
-    <t>Kovacs</t>
-  </si>
-  <si>
-    <t>Sort - A8</t>
-  </si>
-  <si>
-    <t>Donnely</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Catherine</t>
-  </si>
-  <si>
-    <t>Knox</t>
-  </si>
-  <si>
-    <t>Flow Control - A8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ross</t>
-  </si>
-  <si>
-    <t>Izod</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Rukhmani</t>
   </si>
   <si>
     <t>Reddy</t>
-  </si>
-  <si>
-    <t>Flow Control - A9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dale </t>
-  </si>
-  <si>
-    <t>Driscoll</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vickee</t>
-  </si>
-  <si>
-    <t>Anderson</t>
-  </si>
-  <si>
-    <t>Flow Control - A10</t>
-  </si>
-  <si>
-    <t>Skrove</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mary-Ann</t>
-  </si>
-  <si>
-    <t>Korthals</t>
-  </si>
-  <si>
-    <t>Flow Control - A11</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tim</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sylvia</t>
-  </si>
-  <si>
-    <t>Friedrich</t>
-  </si>
-  <si>
-    <t>Fill - A12</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Karen</t>
-  </si>
-  <si>
-    <t>Lohse</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Barb</t>
-  </si>
-  <si>
-    <t>Tyrrell</t>
-  </si>
-  <si>
-    <t>Fill - A13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rick</t>
-  </si>
-  <si>
-    <t>Sehn</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ramji</t>
-  </si>
-  <si>
-    <t>Badhan</t>
-  </si>
-  <si>
-    <t>Fill - A14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kathy</t>
-  </si>
-  <si>
-    <t>Yates</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gurpal </t>
-  </si>
-  <si>
-    <t>Nijjar</t>
-  </si>
-  <si>
-    <t>Fill - A15</t>
-  </si>
-  <si>
-    <t>Silvester</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sohan</t>
   </si>
 </sst>
 </file>
@@ -845,7 +737,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -915,16 +807,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -935,16 +827,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -955,13 +847,13 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -975,13 +867,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -995,16 +887,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1015,13 +907,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -1035,16 +927,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1055,13 +947,13 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -1075,13 +967,13 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -1095,19 +987,19 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -1115,16 +1007,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1135,19 +1027,19 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
         <v>11</v>
@@ -1155,13 +1047,13 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -1175,19 +1067,19 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -1195,16 +1087,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1215,19 +1107,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
         <v>11</v>
@@ -1235,19 +1127,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
         <v>11</v>
@@ -1255,19 +1147,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
         <v>11</v>
@@ -1275,19 +1167,19 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
@@ -1295,19 +1187,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
@@ -1315,19 +1207,19 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
         <v>11</v>
@@ -1335,19 +1227,19 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
@@ -1355,16 +1247,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1375,13 +1267,13 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -1395,13 +1287,13 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
@@ -1415,13 +1307,13 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -1435,13 +1327,13 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
@@ -1455,19 +1347,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F31" t="s">
         <v>11</v>
@@ -1475,19 +1367,19 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F32" t="s">
         <v>11</v>
@@ -1498,16 +1390,16 @@
         <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F33" t="s">
         <v>11</v>
@@ -1515,19 +1407,19 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
         <v>11</v>
@@ -1538,16 +1430,16 @@
         <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F35" t="s">
         <v>11</v>
@@ -1555,19 +1447,19 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
         <v>11</v>
@@ -1578,16 +1470,16 @@
         <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
         <v>11</v>
@@ -1595,19 +1487,19 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F38" t="s">
         <v>11</v>
@@ -1618,16 +1510,16 @@
         <v>96</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
         <v>11</v>
@@ -1635,19 +1527,19 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F40" t="s">
         <v>11</v>
@@ -1658,16 +1550,16 @@
         <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E41" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F41" t="s">
         <v>11</v>
@@ -1675,19 +1567,19 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
         <v>11</v>
@@ -1695,19 +1587,19 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
         <v>107</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E43" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F43" t="s">
         <v>11</v>
@@ -1715,19 +1607,19 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
         <v>11</v>
@@ -1735,19 +1627,19 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E45" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
         <v>11</v>
@@ -1755,19 +1647,19 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="D46" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F46" t="s">
         <v>11</v>
@@ -1775,19 +1667,19 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
         <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E47" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F47" t="s">
         <v>11</v>
@@ -1795,19 +1687,19 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C48" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
@@ -1815,19 +1707,19 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C49" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E49" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F49" t="s">
         <v>11</v>
@@ -1835,19 +1727,19 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B50" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D50" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F50" t="s">
         <v>11</v>
@@ -1855,361 +1747,21 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F51" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" t="s">
-        <v>124</v>
-      </c>
-      <c r="B52" t="s">
-        <v>126</v>
-      </c>
-      <c r="C52" t="s">
-        <v>127</v>
-      </c>
-      <c r="D52" t="s">
-        <v>14</v>
-      </c>
-      <c r="E52" t="s">
-        <v>36</v>
-      </c>
-      <c r="F52" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" t="s">
-        <v>130</v>
-      </c>
-      <c r="D53" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" t="s">
-        <v>36</v>
-      </c>
-      <c r="F53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>128</v>
-      </c>
-      <c r="B54" t="s">
-        <v>131</v>
-      </c>
-      <c r="C54" t="s">
-        <v>132</v>
-      </c>
-      <c r="D54" t="s">
-        <v>14</v>
-      </c>
-      <c r="E54" t="s">
-        <v>36</v>
-      </c>
-      <c r="F54" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B55" t="s">
-        <v>134</v>
-      </c>
-      <c r="C55" t="s">
-        <v>135</v>
-      </c>
-      <c r="D55" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" t="s">
-        <v>36</v>
-      </c>
-      <c r="F55" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" t="s">
-        <v>133</v>
-      </c>
-      <c r="B56" t="s">
-        <v>136</v>
-      </c>
-      <c r="C56" t="s">
-        <v>137</v>
-      </c>
-      <c r="D56" t="s">
-        <v>14</v>
-      </c>
-      <c r="E56" t="s">
-        <v>36</v>
-      </c>
-      <c r="F56" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>138</v>
-      </c>
-      <c r="B57" t="s">
-        <v>99</v>
-      </c>
-      <c r="C57" t="s">
-        <v>139</v>
-      </c>
-      <c r="D57" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" t="s">
-        <v>36</v>
-      </c>
-      <c r="F57" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" t="s">
-        <v>138</v>
-      </c>
-      <c r="B58" t="s">
-        <v>140</v>
-      </c>
-      <c r="C58" t="s">
-        <v>141</v>
-      </c>
-      <c r="D58" t="s">
-        <v>14</v>
-      </c>
-      <c r="E58" t="s">
-        <v>36</v>
-      </c>
-      <c r="F58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" t="s">
-        <v>142</v>
-      </c>
-      <c r="B59" t="s">
-        <v>143</v>
-      </c>
-      <c r="C59" t="s">
-        <v>139</v>
-      </c>
-      <c r="D59" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" t="s">
-        <v>36</v>
-      </c>
-      <c r="F59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>142</v>
-      </c>
-      <c r="B60" t="s">
-        <v>144</v>
-      </c>
-      <c r="C60" t="s">
-        <v>145</v>
-      </c>
-      <c r="D60" t="s">
-        <v>14</v>
-      </c>
-      <c r="E60" t="s">
-        <v>36</v>
-      </c>
-      <c r="F60" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>146</v>
-      </c>
-      <c r="B61" t="s">
-        <v>147</v>
-      </c>
-      <c r="C61" t="s">
-        <v>148</v>
-      </c>
-      <c r="D61" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" t="s">
-        <v>36</v>
-      </c>
-      <c r="F61" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" t="s">
-        <v>146</v>
-      </c>
-      <c r="B62" t="s">
-        <v>149</v>
-      </c>
-      <c r="C62" t="s">
-        <v>150</v>
-      </c>
-      <c r="D62" t="s">
-        <v>14</v>
-      </c>
-      <c r="E62" t="s">
-        <v>36</v>
-      </c>
-      <c r="F62" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="s">
-        <v>151</v>
-      </c>
-      <c r="B63" t="s">
-        <v>152</v>
-      </c>
-      <c r="C63" t="s">
-        <v>153</v>
-      </c>
-      <c r="D63" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" t="s">
-        <v>36</v>
-      </c>
-      <c r="F63" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
-        <v>151</v>
-      </c>
-      <c r="B64" t="s">
-        <v>154</v>
-      </c>
-      <c r="C64" t="s">
-        <v>155</v>
-      </c>
-      <c r="D64" t="s">
-        <v>14</v>
-      </c>
-      <c r="E64" t="s">
-        <v>36</v>
-      </c>
-      <c r="F64" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
-        <v>156</v>
-      </c>
-      <c r="B65" t="s">
-        <v>157</v>
-      </c>
-      <c r="C65" t="s">
-        <v>158</v>
-      </c>
-      <c r="D65" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" t="s">
-        <v>36</v>
-      </c>
-      <c r="F65" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
-        <v>156</v>
-      </c>
-      <c r="B66" t="s">
-        <v>159</v>
-      </c>
-      <c r="C66" t="s">
-        <v>160</v>
-      </c>
-      <c r="D66" t="s">
-        <v>14</v>
-      </c>
-      <c r="E66" t="s">
-        <v>36</v>
-      </c>
-      <c r="F66" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" t="s">
-        <v>161</v>
-      </c>
-      <c r="B67" t="s">
-        <v>149</v>
-      </c>
-      <c r="C67" t="s">
-        <v>162</v>
-      </c>
-      <c r="D67" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" t="s">
-        <v>36</v>
-      </c>
-      <c r="F67" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" t="s">
-        <v>161</v>
-      </c>
-      <c r="B68" t="s">
-        <v>163</v>
-      </c>
-      <c r="C68" t="s">
-        <v>65</v>
-      </c>
-      <c r="D68" t="s">
-        <v>14</v>
-      </c>
-      <c r="E68" t="s">
-        <v>36</v>
-      </c>
-      <c r="F68" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
schedule will now show position/shifts that could not find a person for
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -80,6 +80,9 @@
     <t>Palletizer</t>
   </si>
   <si>
+    <t>UNFILLED POSITION</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Javed</t>
   </si>
   <si>
@@ -228,9 +231,6 @@
   </si>
   <si>
     <t>Sort - A5</t>
-  </si>
-  <si>
-    <t>UNFILLED POSITION</t>
   </si>
   <si>
     <t xml:space="preserve"> George C</t>
@@ -853,10 +853,10 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -867,13 +867,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -887,16 +887,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -907,13 +907,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -927,13 +927,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -947,13 +947,13 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -967,13 +967,13 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -987,13 +987,13 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -1007,13 +1007,13 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -1027,13 +1027,13 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -1047,13 +1047,13 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -1067,13 +1067,13 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
@@ -1087,13 +1087,13 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -1107,13 +1107,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
         <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -1127,13 +1127,13 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -1147,13 +1147,13 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
         <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>59</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
@@ -1167,13 +1167,13 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -1187,13 +1187,13 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
         <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" t="s">
-        <v>64</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
@@ -1207,13 +1207,13 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
@@ -1227,13 +1227,13 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
         <v>65</v>
-      </c>
-      <c r="B25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -1247,16 +1247,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1267,16 +1267,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
         <v>70</v>
       </c>
-      <c r="B27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1287,16 +1287,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1307,16 +1307,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1330,13 +1330,13 @@
         <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1347,16 +1347,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1653,7 +1653,7 @@
         <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
changed card look to 9 columns.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -7,9 +7,8 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Production" sheetId="1" r:id="rId4"/>
-    <sheet name="Sorting" sheetId="2" r:id="rId5"/>
-    <sheet name="Operations" sheetId="3" r:id="rId6"/>
+    <sheet name="Card Display" sheetId="1" r:id="rId4"/>
+    <sheet name="List Display" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -1984,15 +1983,15 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ265"/>
+  <dimension ref="A1:AS265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AJ5" sqref="AJ5"/>
+      <selection activeCell="AK5" sqref="AK5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:45">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2013,41 +2012,43 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="8" t="s">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="17" t="s">
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="AB2" s="10"/>
       <c r="AC2" s="10"/>
       <c r="AD2" s="10"/>
       <c r="AE2" s="10"/>
       <c r="AF2" s="10"/>
       <c r="AG2" s="10"/>
       <c r="AH2" s="10"/>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="17" t="s">
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="AK2" s="10"/>
       <c r="AL2" s="10"/>
       <c r="AM2" s="10"/>
       <c r="AN2" s="10"/>
       <c r="AO2" s="10"/>
       <c r="AP2" s="10"/>
-      <c r="AQ2" s="13"/>
-    </row>
-    <row r="3" spans="1:43">
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="13"/>
+    </row>
+    <row r="3" spans="1:45">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2064,35 +2065,37 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="3"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="11"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="12"/>
       <c r="AC3" s="11"/>
       <c r="AD3" s="11"/>
       <c r="AE3" s="11"/>
       <c r="AF3" s="11"/>
       <c r="AG3" s="11"/>
       <c r="AH3" s="11"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="11"/>
+      <c r="AI3" s="11"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="12"/>
       <c r="AL3" s="11"/>
       <c r="AM3" s="11"/>
       <c r="AN3" s="11"/>
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
-      <c r="AQ3" s="14"/>
-    </row>
-    <row r="5" spans="1:43">
+      <c r="AQ3" s="11"/>
+      <c r="AR3" s="11"/>
+      <c r="AS3" s="14"/>
+    </row>
+    <row r="5" spans="1:45">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -2113,41 +2116,43 @@
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="9" t="s">
+      <c r="Q5" s="6"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="18" t="s">
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AB5" s="15"/>
       <c r="AC5" s="15"/>
       <c r="AD5" s="15"/>
       <c r="AE5" s="15"/>
       <c r="AF5" s="15"/>
       <c r="AG5" s="15"/>
       <c r="AH5" s="15"/>
-      <c r="AI5" s="16"/>
-      <c r="AJ5" s="18" t="s">
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="16"/>
+      <c r="AK5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AK5" s="15"/>
       <c r="AL5" s="15"/>
       <c r="AM5" s="15"/>
       <c r="AN5" s="15"/>
       <c r="AO5" s="15"/>
       <c r="AP5" s="15"/>
-      <c r="AQ5" s="16"/>
-    </row>
-    <row r="7" spans="1:43">
+      <c r="AQ5" s="15"/>
+      <c r="AR5" s="15"/>
+      <c r="AS5" s="16"/>
+    </row>
+    <row r="7" spans="1:45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2167,7 +2172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:45">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2187,7 +2192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:45">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2207,7 +2212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:45">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2227,7 +2232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:45">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2247,7 +2252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:43">
+    <row r="12" spans="1:45">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2267,7 +2272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:45">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2287,7 +2292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:43">
+    <row r="14" spans="1:45">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2307,7 +2312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:43">
+    <row r="15" spans="1:45">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2327,7 +2332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:43">
+    <row r="16" spans="1:45">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2347,7 +2352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:45">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2367,7 +2372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:45">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2387,7 +2392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:45">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2407,7 +2412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:45">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2427,7 +2432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:45">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2447,7 +2452,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:45">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2467,7 +2472,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:43">
+    <row r="23" spans="1:45">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2487,7 +2492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:43">
+    <row r="24" spans="1:45">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2507,7 +2512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:43">
+    <row r="25" spans="1:45">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -2527,7 +2532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:43">
+    <row r="26" spans="1:45">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2547,7 +2552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:45">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -2567,7 +2572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:43">
+    <row r="28" spans="1:45">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -2587,7 +2592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:43">
+    <row r="29" spans="1:45">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -2607,7 +2612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:43">
+    <row r="30" spans="1:45">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -2627,7 +2632,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:43">
+    <row r="31" spans="1:45">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -2647,7 +2652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:43">
+    <row r="32" spans="1:45">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2667,7 +2672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:43">
+    <row r="33" spans="1:45">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -2687,7 +2692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:43">
+    <row r="34" spans="1:45">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2707,7 +2712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:43">
+    <row r="35" spans="1:45">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -2727,7 +2732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:43">
+    <row r="36" spans="1:45">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2747,7 +2752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:43">
+    <row r="37" spans="1:45">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -2767,7 +2772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:43">
+    <row r="38" spans="1:45">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -2787,7 +2792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:43">
+    <row r="39" spans="1:45">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -2807,7 +2812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:43">
+    <row r="40" spans="1:45">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -2827,7 +2832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:43">
+    <row r="41" spans="1:45">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -2847,7 +2852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:43">
+    <row r="42" spans="1:45">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -2867,7 +2872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:43">
+    <row r="43" spans="1:45">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -2887,7 +2892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:43">
+    <row r="44" spans="1:45">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -2907,7 +2912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:43">
+    <row r="45" spans="1:45">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -2927,7 +2932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:43">
+    <row r="46" spans="1:45">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -2947,7 +2952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:43">
+    <row r="47" spans="1:45">
       <c r="A47" t="s">
         <v>68</v>
       </c>
@@ -2967,7 +2972,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:43">
+    <row r="48" spans="1:45">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -2987,7 +2992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:43">
+    <row r="49" spans="1:45">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -3007,7 +3012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:43">
+    <row r="50" spans="1:45">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -3027,7 +3032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:43">
+    <row r="51" spans="1:45">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -3047,7 +3052,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:43">
+    <row r="52" spans="1:45">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -3067,7 +3072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:43">
+    <row r="53" spans="1:45">
       <c r="A53" t="s">
         <v>79</v>
       </c>
@@ -3087,7 +3092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:43">
+    <row r="54" spans="1:45">
       <c r="A54" t="s">
         <v>92</v>
       </c>
@@ -3107,7 +3112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:43">
+    <row r="55" spans="1:45">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -3127,7 +3132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:43">
+    <row r="56" spans="1:45">
       <c r="A56" t="s">
         <v>92</v>
       </c>
@@ -3147,7 +3152,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:43">
+    <row r="57" spans="1:45">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -3167,7 +3172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:43">
+    <row r="58" spans="1:45">
       <c r="A58" t="s">
         <v>92</v>
       </c>
@@ -3187,7 +3192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:43">
+    <row r="59" spans="1:45">
       <c r="A59" t="s">
         <v>92</v>
       </c>
@@ -3207,7 +3212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:43">
+    <row r="60" spans="1:45">
       <c r="A60" t="s">
         <v>103</v>
       </c>
@@ -3227,7 +3232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:43">
+    <row r="61" spans="1:45">
       <c r="A61" t="s">
         <v>103</v>
       </c>
@@ -3247,7 +3252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:43">
+    <row r="62" spans="1:45">
       <c r="A62" t="s">
         <v>103</v>
       </c>
@@ -3267,7 +3272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:43">
+    <row r="63" spans="1:45">
       <c r="A63" t="s">
         <v>103</v>
       </c>
@@ -3287,7 +3292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:43">
+    <row r="64" spans="1:45">
       <c r="A64" t="s">
         <v>103</v>
       </c>
@@ -3307,7 +3312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:43">
+    <row r="65" spans="1:45">
       <c r="A65" t="s">
         <v>103</v>
       </c>
@@ -3327,7 +3332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:43">
+    <row r="66" spans="1:45">
       <c r="A66" t="s">
         <v>115</v>
       </c>
@@ -3347,7 +3352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:43">
+    <row r="67" spans="1:45">
       <c r="A67" t="s">
         <v>115</v>
       </c>
@@ -3367,7 +3372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:43">
+    <row r="68" spans="1:45">
       <c r="A68" t="s">
         <v>115</v>
       </c>
@@ -3387,7 +3392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:43">
+    <row r="69" spans="1:45">
       <c r="A69" t="s">
         <v>115</v>
       </c>
@@ -3407,7 +3412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:43">
+    <row r="70" spans="1:45">
       <c r="A70" t="s">
         <v>115</v>
       </c>
@@ -3427,7 +3432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:43">
+    <row r="71" spans="1:45">
       <c r="A71" t="s">
         <v>115</v>
       </c>
@@ -3447,7 +3452,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:43">
+    <row r="72" spans="1:45">
       <c r="A72" t="s">
         <v>127</v>
       </c>
@@ -3467,7 +3472,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:43">
+    <row r="73" spans="1:45">
       <c r="A73" t="s">
         <v>127</v>
       </c>
@@ -3487,7 +3492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:43">
+    <row r="74" spans="1:45">
       <c r="A74" t="s">
         <v>127</v>
       </c>
@@ -3507,7 +3512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:43">
+    <row r="75" spans="1:45">
       <c r="A75" t="s">
         <v>127</v>
       </c>
@@ -3527,7 +3532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:43">
+    <row r="76" spans="1:45">
       <c r="A76" t="s">
         <v>127</v>
       </c>
@@ -3547,7 +3552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:43">
+    <row r="77" spans="1:45">
       <c r="A77" t="s">
         <v>127</v>
       </c>
@@ -3567,7 +3572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:43">
+    <row r="78" spans="1:45">
       <c r="A78" t="s">
         <v>137</v>
       </c>
@@ -3587,7 +3592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:43">
+    <row r="79" spans="1:45">
       <c r="A79" t="s">
         <v>137</v>
       </c>
@@ -3607,7 +3612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:43">
+    <row r="80" spans="1:45">
       <c r="A80" t="s">
         <v>137</v>
       </c>
@@ -3627,7 +3632,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:43">
+    <row r="81" spans="1:45">
       <c r="A81" t="s">
         <v>137</v>
       </c>
@@ -3647,7 +3652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:43">
+    <row r="82" spans="1:45">
       <c r="A82" t="s">
         <v>137</v>
       </c>
@@ -3667,7 +3672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:43">
+    <row r="83" spans="1:45">
       <c r="A83" t="s">
         <v>137</v>
       </c>
@@ -3687,7 +3692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:43">
+    <row r="84" spans="1:45">
       <c r="A84" t="s">
         <v>148</v>
       </c>
@@ -3707,7 +3712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:43">
+    <row r="85" spans="1:45">
       <c r="A85" t="s">
         <v>148</v>
       </c>
@@ -3727,7 +3732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:43">
+    <row r="86" spans="1:45">
       <c r="A86" t="s">
         <v>148</v>
       </c>
@@ -3747,7 +3752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:43">
+    <row r="87" spans="1:45">
       <c r="A87" t="s">
         <v>148</v>
       </c>
@@ -3767,7 +3772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:43">
+    <row r="88" spans="1:45">
       <c r="A88" t="s">
         <v>148</v>
       </c>
@@ -3787,7 +3792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:43">
+    <row r="89" spans="1:45">
       <c r="A89" t="s">
         <v>148</v>
       </c>
@@ -3807,7 +3812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:43">
+    <row r="90" spans="1:45">
       <c r="A90" t="s">
         <v>160</v>
       </c>
@@ -3827,7 +3832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:43">
+    <row r="91" spans="1:45">
       <c r="A91" t="s">
         <v>160</v>
       </c>
@@ -3847,7 +3852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:43">
+    <row r="92" spans="1:45">
       <c r="A92" t="s">
         <v>160</v>
       </c>
@@ -3867,7 +3872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:43">
+    <row r="93" spans="1:45">
       <c r="A93" t="s">
         <v>160</v>
       </c>
@@ -3887,7 +3892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:43">
+    <row r="94" spans="1:45">
       <c r="A94" t="s">
         <v>160</v>
       </c>
@@ -3907,7 +3912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:43">
+    <row r="95" spans="1:45">
       <c r="A95" t="s">
         <v>160</v>
       </c>
@@ -3927,7 +3932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:43">
+    <row r="96" spans="1:45">
       <c r="A96" t="s">
         <v>172</v>
       </c>
@@ -3947,7 +3952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:43">
+    <row r="97" spans="1:45">
       <c r="A97" t="s">
         <v>172</v>
       </c>
@@ -3967,7 +3972,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:43">
+    <row r="98" spans="1:45">
       <c r="A98" t="s">
         <v>172</v>
       </c>
@@ -3987,7 +3992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:43">
+    <row r="99" spans="1:45">
       <c r="A99" t="s">
         <v>172</v>
       </c>
@@ -4007,7 +4012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:43">
+    <row r="100" spans="1:45">
       <c r="A100" t="s">
         <v>172</v>
       </c>
@@ -4027,7 +4032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:43">
+    <row r="101" spans="1:45">
       <c r="A101" t="s">
         <v>172</v>
       </c>
@@ -4047,7 +4052,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:43">
+    <row r="102" spans="1:45">
       <c r="A102" t="s">
         <v>185</v>
       </c>
@@ -4067,7 +4072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:43">
+    <row r="103" spans="1:45">
       <c r="A103" t="s">
         <v>185</v>
       </c>
@@ -4087,7 +4092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:43">
+    <row r="104" spans="1:45">
       <c r="A104" t="s">
         <v>185</v>
       </c>
@@ -4107,7 +4112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:43">
+    <row r="105" spans="1:45">
       <c r="A105" t="s">
         <v>185</v>
       </c>
@@ -4127,7 +4132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:43">
+    <row r="106" spans="1:45">
       <c r="A106" t="s">
         <v>185</v>
       </c>
@@ -4147,7 +4152,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="107" spans="1:43">
+    <row r="107" spans="1:45">
       <c r="A107" t="s">
         <v>185</v>
       </c>
@@ -4167,7 +4172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="108" spans="1:43">
+    <row r="108" spans="1:45">
       <c r="A108" t="s">
         <v>198</v>
       </c>
@@ -4187,7 +4192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:43">
+    <row r="109" spans="1:45">
       <c r="A109" t="s">
         <v>198</v>
       </c>
@@ -4207,7 +4212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="110" spans="1:43">
+    <row r="110" spans="1:45">
       <c r="A110" t="s">
         <v>198</v>
       </c>
@@ -4227,7 +4232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:43">
+    <row r="111" spans="1:45">
       <c r="A111" t="s">
         <v>198</v>
       </c>
@@ -4247,7 +4252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="1:43">
+    <row r="112" spans="1:45">
       <c r="A112" t="s">
         <v>198</v>
       </c>
@@ -4267,7 +4272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:43">
+    <row r="113" spans="1:45">
       <c r="A113" t="s">
         <v>198</v>
       </c>
@@ -4287,7 +4292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="1:43">
+    <row r="114" spans="1:45">
       <c r="A114" t="s">
         <v>210</v>
       </c>
@@ -4307,7 +4312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:43">
+    <row r="115" spans="1:45">
       <c r="A115" t="s">
         <v>210</v>
       </c>
@@ -4327,7 +4332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="116" spans="1:43">
+    <row r="116" spans="1:45">
       <c r="A116" t="s">
         <v>210</v>
       </c>
@@ -4347,7 +4352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="117" spans="1:43">
+    <row r="117" spans="1:45">
       <c r="A117" t="s">
         <v>210</v>
       </c>
@@ -4367,7 +4372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:43">
+    <row r="118" spans="1:45">
       <c r="A118" t="s">
         <v>210</v>
       </c>
@@ -4387,7 +4392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="119" spans="1:43">
+    <row r="119" spans="1:45">
       <c r="A119" t="s">
         <v>210</v>
       </c>
@@ -4407,7 +4412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" spans="1:43">
+    <row r="120" spans="1:45">
       <c r="A120" t="s">
         <v>221</v>
       </c>
@@ -4427,7 +4432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="121" spans="1:43">
+    <row r="121" spans="1:45">
       <c r="A121" t="s">
         <v>221</v>
       </c>
@@ -4447,7 +4452,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" spans="1:43">
+    <row r="122" spans="1:45">
       <c r="A122" t="s">
         <v>221</v>
       </c>
@@ -4467,7 +4472,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:43">
+    <row r="123" spans="1:45">
       <c r="A123" t="s">
         <v>221</v>
       </c>
@@ -4487,7 +4492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="124" spans="1:43">
+    <row r="124" spans="1:45">
       <c r="A124" t="s">
         <v>221</v>
       </c>
@@ -4507,7 +4512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="125" spans="1:43">
+    <row r="125" spans="1:45">
       <c r="A125" t="s">
         <v>221</v>
       </c>
@@ -4527,7 +4532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="126" spans="1:43">
+    <row r="126" spans="1:45">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -4547,7 +4552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:43">
+    <row r="127" spans="1:45">
       <c r="A127" t="s">
         <v>233</v>
       </c>
@@ -4567,7 +4572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="128" spans="1:43">
+    <row r="128" spans="1:45">
       <c r="A128" t="s">
         <v>233</v>
       </c>
@@ -4587,7 +4592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="129" spans="1:43">
+    <row r="129" spans="1:45">
       <c r="A129" t="s">
         <v>233</v>
       </c>
@@ -4607,7 +4612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="130" spans="1:43">
+    <row r="130" spans="1:45">
       <c r="A130" t="s">
         <v>233</v>
       </c>
@@ -4627,7 +4632,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="131" spans="1:43">
+    <row r="131" spans="1:45">
       <c r="A131" t="s">
         <v>233</v>
       </c>
@@ -4647,7 +4652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="132" spans="1:43">
+    <row r="132" spans="1:45">
       <c r="A132" t="s">
         <v>245</v>
       </c>
@@ -4667,7 +4672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="133" spans="1:43">
+    <row r="133" spans="1:45">
       <c r="A133" t="s">
         <v>245</v>
       </c>
@@ -4687,7 +4692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:43">
+    <row r="134" spans="1:45">
       <c r="A134" t="s">
         <v>245</v>
       </c>
@@ -4707,7 +4712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="1:43">
+    <row r="135" spans="1:45">
       <c r="A135" t="s">
         <v>245</v>
       </c>
@@ -4727,7 +4732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="136" spans="1:43">
+    <row r="136" spans="1:45">
       <c r="A136" t="s">
         <v>245</v>
       </c>
@@ -4747,7 +4752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:43">
+    <row r="137" spans="1:45">
       <c r="A137" t="s">
         <v>245</v>
       </c>
@@ -4767,7 +4772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="138" spans="1:43">
+    <row r="138" spans="1:45">
       <c r="A138" t="s">
         <v>256</v>
       </c>
@@ -4787,7 +4792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" spans="1:43">
+    <row r="139" spans="1:45">
       <c r="A139" t="s">
         <v>256</v>
       </c>
@@ -4807,7 +4812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="140" spans="1:43">
+    <row r="140" spans="1:45">
       <c r="A140" t="s">
         <v>256</v>
       </c>
@@ -4827,7 +4832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="141" spans="1:43">
+    <row r="141" spans="1:45">
       <c r="A141" t="s">
         <v>256</v>
       </c>
@@ -4847,7 +4852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="142" spans="1:43">
+    <row r="142" spans="1:45">
       <c r="A142" t="s">
         <v>256</v>
       </c>
@@ -4867,7 +4872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="143" spans="1:43">
+    <row r="143" spans="1:45">
       <c r="A143" t="s">
         <v>256</v>
       </c>
@@ -4887,7 +4892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="144" spans="1:43">
+    <row r="144" spans="1:45">
       <c r="A144" t="s">
         <v>266</v>
       </c>
@@ -4907,7 +4912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="145" spans="1:43">
+    <row r="145" spans="1:45">
       <c r="A145" t="s">
         <v>266</v>
       </c>
@@ -4927,7 +4932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="1:43">
+    <row r="146" spans="1:45">
       <c r="A146" t="s">
         <v>266</v>
       </c>
@@ -4947,7 +4952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="147" spans="1:43">
+    <row r="147" spans="1:45">
       <c r="A147" t="s">
         <v>266</v>
       </c>
@@ -4967,7 +4972,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="148" spans="1:43">
+    <row r="148" spans="1:45">
       <c r="A148" t="s">
         <v>266</v>
       </c>
@@ -4987,7 +4992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="149" spans="1:43">
+    <row r="149" spans="1:45">
       <c r="A149" t="s">
         <v>266</v>
       </c>
@@ -5007,7 +5012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="150" spans="1:43">
+    <row r="150" spans="1:45">
       <c r="A150" t="s">
         <v>276</v>
       </c>
@@ -5027,7 +5032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="1:43">
+    <row r="151" spans="1:45">
       <c r="A151" t="s">
         <v>276</v>
       </c>
@@ -5047,7 +5052,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" spans="1:43">
+    <row r="152" spans="1:45">
       <c r="A152" t="s">
         <v>276</v>
       </c>
@@ -5067,7 +5072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="153" spans="1:43">
+    <row r="153" spans="1:45">
       <c r="A153" t="s">
         <v>276</v>
       </c>
@@ -5087,7 +5092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" spans="1:43">
+    <row r="154" spans="1:45">
       <c r="A154" t="s">
         <v>276</v>
       </c>
@@ -5107,7 +5112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:43">
+    <row r="155" spans="1:45">
       <c r="A155" t="s">
         <v>276</v>
       </c>
@@ -5127,7 +5132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:43">
+    <row r="156" spans="1:45">
       <c r="A156" t="s">
         <v>287</v>
       </c>
@@ -5147,7 +5152,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="157" spans="1:43">
+    <row r="157" spans="1:45">
       <c r="A157" t="s">
         <v>287</v>
       </c>
@@ -5167,7 +5172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="158" spans="1:43">
+    <row r="158" spans="1:45">
       <c r="A158" t="s">
         <v>287</v>
       </c>
@@ -5187,7 +5192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="159" spans="1:43">
+    <row r="159" spans="1:45">
       <c r="A159" t="s">
         <v>287</v>
       </c>
@@ -5207,7 +5212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="160" spans="1:43">
+    <row r="160" spans="1:45">
       <c r="A160" t="s">
         <v>287</v>
       </c>
@@ -5227,7 +5232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="161" spans="1:43">
+    <row r="161" spans="1:45">
       <c r="A161" t="s">
         <v>287</v>
       </c>
@@ -5247,7 +5252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" spans="1:43">
+    <row r="162" spans="1:45">
       <c r="A162" t="s">
         <v>299</v>
       </c>
@@ -5267,7 +5272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="163" spans="1:43">
+    <row r="163" spans="1:45">
       <c r="A163" t="s">
         <v>299</v>
       </c>
@@ -5287,7 +5292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" spans="1:43">
+    <row r="164" spans="1:45">
       <c r="A164" t="s">
         <v>299</v>
       </c>
@@ -5307,7 +5312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="165" spans="1:43">
+    <row r="165" spans="1:45">
       <c r="A165" t="s">
         <v>299</v>
       </c>
@@ -5327,7 +5332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="166" spans="1:43">
+    <row r="166" spans="1:45">
       <c r="A166" t="s">
         <v>299</v>
       </c>
@@ -5347,7 +5352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="167" spans="1:43">
+    <row r="167" spans="1:45">
       <c r="A167" t="s">
         <v>299</v>
       </c>
@@ -5367,7 +5372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="168" spans="1:43">
+    <row r="168" spans="1:45">
       <c r="A168" t="s">
         <v>311</v>
       </c>
@@ -5387,7 +5392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="169" spans="1:43">
+    <row r="169" spans="1:45">
       <c r="A169" t="s">
         <v>311</v>
       </c>
@@ -5407,7 +5412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" spans="1:43">
+    <row r="170" spans="1:45">
       <c r="A170" t="s">
         <v>311</v>
       </c>
@@ -5427,7 +5432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="171" spans="1:43">
+    <row r="171" spans="1:45">
       <c r="A171" t="s">
         <v>311</v>
       </c>
@@ -5447,7 +5452,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="172" spans="1:43">
+    <row r="172" spans="1:45">
       <c r="A172" t="s">
         <v>311</v>
       </c>
@@ -5467,7 +5472,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="173" spans="1:43">
+    <row r="173" spans="1:45">
       <c r="A173" t="s">
         <v>311</v>
       </c>
@@ -5487,7 +5492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="174" spans="1:43">
+    <row r="174" spans="1:45">
       <c r="A174" t="s">
         <v>324</v>
       </c>
@@ -5507,7 +5512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="175" spans="1:43">
+    <row r="175" spans="1:45">
       <c r="A175" t="s">
         <v>324</v>
       </c>
@@ -5527,7 +5532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="176" spans="1:43">
+    <row r="176" spans="1:45">
       <c r="A176" t="s">
         <v>324</v>
       </c>
@@ -5547,7 +5552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="177" spans="1:43">
+    <row r="177" spans="1:45">
       <c r="A177" t="s">
         <v>324</v>
       </c>
@@ -5567,7 +5572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="178" spans="1:43">
+    <row r="178" spans="1:45">
       <c r="A178" t="s">
         <v>324</v>
       </c>
@@ -5587,7 +5592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="179" spans="1:43">
+    <row r="179" spans="1:45">
       <c r="A179" t="s">
         <v>324</v>
       </c>
@@ -5607,7 +5612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="180" spans="1:43">
+    <row r="180" spans="1:45">
       <c r="A180" t="s">
         <v>336</v>
       </c>
@@ -5627,7 +5632,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="181" spans="1:43">
+    <row r="181" spans="1:45">
       <c r="A181" t="s">
         <v>336</v>
       </c>
@@ -5647,7 +5652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="182" spans="1:43">
+    <row r="182" spans="1:45">
       <c r="A182" t="s">
         <v>336</v>
       </c>
@@ -5667,7 +5672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="183" spans="1:43">
+    <row r="183" spans="1:45">
       <c r="A183" t="s">
         <v>336</v>
       </c>
@@ -5687,7 +5692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="184" spans="1:43">
+    <row r="184" spans="1:45">
       <c r="A184" t="s">
         <v>336</v>
       </c>
@@ -5707,7 +5712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="185" spans="1:43">
+    <row r="185" spans="1:45">
       <c r="A185" t="s">
         <v>336</v>
       </c>
@@ -5727,7 +5732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="186" spans="1:43">
+    <row r="186" spans="1:45">
       <c r="A186" t="s">
         <v>347</v>
       </c>
@@ -5747,7 +5752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="187" spans="1:43">
+    <row r="187" spans="1:45">
       <c r="A187" t="s">
         <v>347</v>
       </c>
@@ -5767,7 +5772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="188" spans="1:43">
+    <row r="188" spans="1:45">
       <c r="A188" t="s">
         <v>347</v>
       </c>
@@ -5787,7 +5792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="189" spans="1:43">
+    <row r="189" spans="1:45">
       <c r="A189" t="s">
         <v>347</v>
       </c>
@@ -5807,7 +5812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="190" spans="1:43">
+    <row r="190" spans="1:45">
       <c r="A190" t="s">
         <v>347</v>
       </c>
@@ -5827,7 +5832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="191" spans="1:43">
+    <row r="191" spans="1:45">
       <c r="A191" t="s">
         <v>347</v>
       </c>
@@ -5847,7 +5852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="192" spans="1:43">
+    <row r="192" spans="1:45">
       <c r="A192" t="s">
         <v>358</v>
       </c>
@@ -5867,7 +5872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="193" spans="1:43">
+    <row r="193" spans="1:45">
       <c r="A193" t="s">
         <v>358</v>
       </c>
@@ -5887,7 +5892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="194" spans="1:43">
+    <row r="194" spans="1:45">
       <c r="A194" t="s">
         <v>358</v>
       </c>
@@ -5907,7 +5912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="195" spans="1:43">
+    <row r="195" spans="1:45">
       <c r="A195" t="s">
         <v>358</v>
       </c>
@@ -5927,7 +5932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="196" spans="1:43">
+    <row r="196" spans="1:45">
       <c r="A196" t="s">
         <v>358</v>
       </c>
@@ -5947,7 +5952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" spans="1:43">
+    <row r="197" spans="1:45">
       <c r="A197" t="s">
         <v>358</v>
       </c>
@@ -5967,7 +5972,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="198" spans="1:43">
+    <row r="198" spans="1:45">
       <c r="A198" t="s">
         <v>370</v>
       </c>
@@ -5987,7 +5992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="199" spans="1:43">
+    <row r="199" spans="1:45">
       <c r="A199" t="s">
         <v>370</v>
       </c>
@@ -6007,7 +6012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="200" spans="1:43">
+    <row r="200" spans="1:45">
       <c r="A200" t="s">
         <v>370</v>
       </c>
@@ -6027,7 +6032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="201" spans="1:43">
+    <row r="201" spans="1:45">
       <c r="A201" t="s">
         <v>370</v>
       </c>
@@ -6047,7 +6052,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="202" spans="1:43">
+    <row r="202" spans="1:45">
       <c r="A202" t="s">
         <v>370</v>
       </c>
@@ -6067,7 +6072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="203" spans="1:43">
+    <row r="203" spans="1:45">
       <c r="A203" t="s">
         <v>370</v>
       </c>
@@ -6087,7 +6092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="204" spans="1:43">
+    <row r="204" spans="1:45">
       <c r="A204" t="s">
         <v>380</v>
       </c>
@@ -6107,7 +6112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="205" spans="1:43">
+    <row r="205" spans="1:45">
       <c r="A205" t="s">
         <v>380</v>
       </c>
@@ -6127,7 +6132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="206" spans="1:43">
+    <row r="206" spans="1:45">
       <c r="A206" t="s">
         <v>380</v>
       </c>
@@ -6147,7 +6152,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="207" spans="1:43">
+    <row r="207" spans="1:45">
       <c r="A207" t="s">
         <v>380</v>
       </c>
@@ -6167,7 +6172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="208" spans="1:43">
+    <row r="208" spans="1:45">
       <c r="A208" t="s">
         <v>380</v>
       </c>
@@ -6187,7 +6192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="209" spans="1:43">
+    <row r="209" spans="1:45">
       <c r="A209" t="s">
         <v>380</v>
       </c>
@@ -6207,7 +6212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="210" spans="1:43">
+    <row r="210" spans="1:45">
       <c r="A210" t="s">
         <v>392</v>
       </c>
@@ -6227,7 +6232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="211" spans="1:43">
+    <row r="211" spans="1:45">
       <c r="A211" t="s">
         <v>392</v>
       </c>
@@ -6247,7 +6252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="212" spans="1:43">
+    <row r="212" spans="1:45">
       <c r="A212" t="s">
         <v>392</v>
       </c>
@@ -6267,7 +6272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="213" spans="1:43">
+    <row r="213" spans="1:45">
       <c r="A213" t="s">
         <v>392</v>
       </c>
@@ -6287,7 +6292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="214" spans="1:43">
+    <row r="214" spans="1:45">
       <c r="A214" t="s">
         <v>392</v>
       </c>
@@ -6307,7 +6312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="215" spans="1:43">
+    <row r="215" spans="1:45">
       <c r="A215" t="s">
         <v>392</v>
       </c>
@@ -6327,7 +6332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="216" spans="1:43">
+    <row r="216" spans="1:45">
       <c r="A216" t="s">
         <v>405</v>
       </c>
@@ -6347,7 +6352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="217" spans="1:43">
+    <row r="217" spans="1:45">
       <c r="A217" t="s">
         <v>405</v>
       </c>
@@ -6367,7 +6372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="218" spans="1:43">
+    <row r="218" spans="1:45">
       <c r="A218" t="s">
         <v>405</v>
       </c>
@@ -6387,7 +6392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="219" spans="1:43">
+    <row r="219" spans="1:45">
       <c r="A219" t="s">
         <v>405</v>
       </c>
@@ -6407,7 +6412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="220" spans="1:43">
+    <row r="220" spans="1:45">
       <c r="A220" t="s">
         <v>405</v>
       </c>
@@ -6427,7 +6432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="221" spans="1:43">
+    <row r="221" spans="1:45">
       <c r="A221" t="s">
         <v>405</v>
       </c>
@@ -6447,7 +6452,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="222" spans="1:43">
+    <row r="222" spans="1:45">
       <c r="A222" t="s">
         <v>417</v>
       </c>
@@ -6467,7 +6472,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="223" spans="1:43">
+    <row r="223" spans="1:45">
       <c r="A223" t="s">
         <v>417</v>
       </c>
@@ -6487,7 +6492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="224" spans="1:43">
+    <row r="224" spans="1:45">
       <c r="A224" t="s">
         <v>417</v>
       </c>
@@ -6507,7 +6512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="225" spans="1:43">
+    <row r="225" spans="1:45">
       <c r="A225" t="s">
         <v>417</v>
       </c>
@@ -6527,7 +6532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="226" spans="1:43">
+    <row r="226" spans="1:45">
       <c r="A226" t="s">
         <v>417</v>
       </c>
@@ -6547,7 +6552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="227" spans="1:43">
+    <row r="227" spans="1:45">
       <c r="A227" t="s">
         <v>417</v>
       </c>
@@ -6567,7 +6572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="228" spans="1:43">
+    <row r="228" spans="1:45">
       <c r="A228" t="s">
         <v>429</v>
       </c>
@@ -6587,7 +6592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="229" spans="1:43">
+    <row r="229" spans="1:45">
       <c r="A229" t="s">
         <v>429</v>
       </c>
@@ -6607,7 +6612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="230" spans="1:43">
+    <row r="230" spans="1:45">
       <c r="A230" t="s">
         <v>429</v>
       </c>
@@ -6627,7 +6632,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="231" spans="1:43">
+    <row r="231" spans="1:45">
       <c r="A231" t="s">
         <v>429</v>
       </c>
@@ -6647,7 +6652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="232" spans="1:43">
+    <row r="232" spans="1:45">
       <c r="A232" t="s">
         <v>429</v>
       </c>
@@ -6667,7 +6672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="233" spans="1:43">
+    <row r="233" spans="1:45">
       <c r="A233" t="s">
         <v>429</v>
       </c>
@@ -6687,7 +6692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="234" spans="1:43">
+    <row r="234" spans="1:45">
       <c r="A234" t="s">
         <v>439</v>
       </c>
@@ -6707,7 +6712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="235" spans="1:43">
+    <row r="235" spans="1:45">
       <c r="A235" t="s">
         <v>439</v>
       </c>
@@ -6727,7 +6732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="236" spans="1:43">
+    <row r="236" spans="1:45">
       <c r="A236" t="s">
         <v>443</v>
       </c>
@@ -6747,7 +6752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="237" spans="1:43">
+    <row r="237" spans="1:45">
       <c r="A237" t="s">
         <v>443</v>
       </c>
@@ -6767,7 +6772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="238" spans="1:43">
+    <row r="238" spans="1:45">
       <c r="A238" t="s">
         <v>443</v>
       </c>
@@ -6787,7 +6792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="239" spans="1:43">
+    <row r="239" spans="1:45">
       <c r="A239" t="s">
         <v>443</v>
       </c>
@@ -6807,7 +6812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="240" spans="1:43">
+    <row r="240" spans="1:45">
       <c r="A240" t="s">
         <v>443</v>
       </c>
@@ -6827,7 +6832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="241" spans="1:43">
+    <row r="241" spans="1:45">
       <c r="A241" t="s">
         <v>443</v>
       </c>
@@ -6847,7 +6852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="242" spans="1:43">
+    <row r="242" spans="1:45">
       <c r="A242" t="s">
         <v>453</v>
       </c>
@@ -6867,7 +6872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="243" spans="1:43">
+    <row r="243" spans="1:45">
       <c r="A243" t="s">
         <v>453</v>
       </c>
@@ -6887,7 +6892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="244" spans="1:43">
+    <row r="244" spans="1:45">
       <c r="A244" t="s">
         <v>453</v>
       </c>
@@ -6907,7 +6912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="245" spans="1:43">
+    <row r="245" spans="1:45">
       <c r="A245" t="s">
         <v>453</v>
       </c>
@@ -6927,7 +6932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="246" spans="1:43">
+    <row r="246" spans="1:45">
       <c r="A246" t="s">
         <v>460</v>
       </c>
@@ -6947,7 +6952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="247" spans="1:43">
+    <row r="247" spans="1:45">
       <c r="A247" t="s">
         <v>460</v>
       </c>
@@ -6967,7 +6972,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="248" spans="1:43">
+    <row r="248" spans="1:45">
       <c r="A248" t="s">
         <v>465</v>
       </c>
@@ -6987,7 +6992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="249" spans="1:43">
+    <row r="249" spans="1:45">
       <c r="A249" t="s">
         <v>465</v>
       </c>
@@ -7007,7 +7012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="250" spans="1:43">
+    <row r="250" spans="1:45">
       <c r="A250" t="s">
         <v>468</v>
       </c>
@@ -7027,7 +7032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="251" spans="1:43">
+    <row r="251" spans="1:45">
       <c r="A251" t="s">
         <v>468</v>
       </c>
@@ -7047,7 +7052,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="252" spans="1:43">
+    <row r="252" spans="1:45">
       <c r="A252" t="s">
         <v>473</v>
       </c>
@@ -7067,7 +7072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="253" spans="1:43">
+    <row r="253" spans="1:45">
       <c r="A253" t="s">
         <v>473</v>
       </c>
@@ -7087,7 +7092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="254" spans="1:43">
+    <row r="254" spans="1:45">
       <c r="A254" t="s">
         <v>477</v>
       </c>
@@ -7107,7 +7112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="255" spans="1:43">
+    <row r="255" spans="1:45">
       <c r="A255" t="s">
         <v>477</v>
       </c>
@@ -7127,7 +7132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="256" spans="1:43">
+    <row r="256" spans="1:45">
       <c r="A256" t="s">
         <v>481</v>
       </c>
@@ -7147,7 +7152,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="257" spans="1:43">
+    <row r="257" spans="1:45">
       <c r="A257" t="s">
         <v>481</v>
       </c>
@@ -7167,7 +7172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="258" spans="1:43">
+    <row r="258" spans="1:45">
       <c r="A258" t="s">
         <v>485</v>
       </c>
@@ -7187,7 +7192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="259" spans="1:43">
+    <row r="259" spans="1:45">
       <c r="A259" t="s">
         <v>485</v>
       </c>
@@ -7207,7 +7212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="260" spans="1:43">
+    <row r="260" spans="1:45">
       <c r="A260" t="s">
         <v>486</v>
       </c>
@@ -7227,7 +7232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="261" spans="1:43">
+    <row r="261" spans="1:45">
       <c r="A261" t="s">
         <v>486</v>
       </c>
@@ -7247,7 +7252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="262" spans="1:43">
+    <row r="262" spans="1:45">
       <c r="A262" t="s">
         <v>487</v>
       </c>
@@ -7267,7 +7272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="263" spans="1:43">
+    <row r="263" spans="1:45">
       <c r="A263" t="s">
         <v>488</v>
       </c>
@@ -7287,7 +7292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="264" spans="1:43">
+    <row r="264" spans="1:45">
       <c r="A264" t="s">
         <v>489</v>
       </c>
@@ -7307,7 +7312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="265" spans="1:43">
+    <row r="265" spans="1:45">
       <c r="A265" t="s">
         <v>490</v>
       </c>
@@ -7332,14 +7337,14 @@
   <mergeCells>
     <mergeCell ref="A2:I3"/>
     <mergeCell ref="A5:I5"/>
-    <mergeCell ref="J2:Q3"/>
-    <mergeCell ref="J5:Q5"/>
-    <mergeCell ref="R2:Z3"/>
-    <mergeCell ref="R5:Z5"/>
-    <mergeCell ref="AA2:AI3"/>
-    <mergeCell ref="AA5:AI5"/>
-    <mergeCell ref="AJ2:AQ3"/>
-    <mergeCell ref="AJ5:AQ5"/>
+    <mergeCell ref="J2:R3"/>
+    <mergeCell ref="J5:R5"/>
+    <mergeCell ref="S2:AA3"/>
+    <mergeCell ref="S5:AA5"/>
+    <mergeCell ref="AB2:AJ3"/>
+    <mergeCell ref="AB5:AJ5"/>
+    <mergeCell ref="AK2:AS3"/>
+    <mergeCell ref="AK5:AS5"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7352,13 +7357,12 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <colBreaks count="6" manualBreakCount="6">
+  <colBreaks count="5" manualBreakCount="5">
     <brk id="9" man="1"/>
-    <brk id="17" man="1"/>
-    <brk id="26" man="1"/>
-    <brk id="35" man="1"/>
-    <brk id="43" man="1"/>
-    <brk id="52" man="1"/>
+    <brk id="18" man="1"/>
+    <brk id="27" man="1"/>
+    <brk id="36" man="1"/>
+    <brk id="45" man="1"/>
   </colBreaks>
 </worksheet>
 </file>
@@ -7389,32 +7393,4 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added variables to display the schedule headers
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Card Display" sheetId="1" r:id="rId4"/>
@@ -67,7 +67,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +89,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAF442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border/>
@@ -168,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -224,6 +230,33 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="4" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -527,7 +560,7 @@
   </sheetPr>
   <dimension ref="A1:AS5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="AK5" sqref="AK5"/>
     </sheetView>
   </sheetViews>
@@ -734,15 +767,123 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:27">
+      <c r="A2" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="22"/>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="21"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="23"/>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="25"/>
+    </row>
+  </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="A2:I3"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="J2:R3"/>
+    <mergeCell ref="J5:R5"/>
+    <mergeCell ref="S2:AA3"/>
+    <mergeCell ref="S5:AA5"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>

</xml_diff>

<commit_message>
added logic for printing day and night together
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -16,13 +16,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+  <si>
+    <t>Friday March 4, 2016</t>
+  </si>
+  <si>
+    <t>Cherry Line Production 7:00AM - 3:30PM</t>
+  </si>
+  <si>
+    <t>Cherry Line Sorting 7:00AM - 3:30PM</t>
+  </si>
+  <si>
+    <t>Operations 7:00AM - 3:30PM</t>
+  </si>
+  <si>
+    <t>Cherry Line Production 4:00PM - 12:30AM</t>
+  </si>
+  <si>
+    <t>Cherry Line Sorting 4:00PM - 12:30AM</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -32,8 +51,26 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -43,16 +80,154 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAF442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3F7FBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border/>
+    <border>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="19">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -353,15 +528,189 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AS5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="AK5" sqref="AK5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:45">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="10"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="13"/>
+    </row>
+    <row r="3" spans="1:45">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="11"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="11"/>
+      <c r="AM3" s="11"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="11"/>
+      <c r="AP3" s="11"/>
+      <c r="AQ3" s="11"/>
+      <c r="AR3" s="11"/>
+      <c r="AS3" s="14"/>
+    </row>
+    <row r="5" spans="1:45">
+      <c r="A5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="16"/>
+      <c r="AK5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="15"/>
+      <c r="AN5" s="15"/>
+      <c r="AO5" s="15"/>
+      <c r="AP5" s="15"/>
+      <c r="AQ5" s="15"/>
+      <c r="AR5" s="15"/>
+      <c r="AS5" s="16"/>
+    </row>
+  </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="A2:I3"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="J2:R3"/>
+    <mergeCell ref="J5:R5"/>
+    <mergeCell ref="S2:AA3"/>
+    <mergeCell ref="S5:AA5"/>
+    <mergeCell ref="AB2:AJ3"/>
+    <mergeCell ref="AB5:AJ5"/>
+    <mergeCell ref="AK2:AS3"/>
+    <mergeCell ref="AK5:AS5"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>

</xml_diff>

<commit_message>
added for loop to iterator through the emps
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -16,24 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
     <t>Friday March 4, 2016</t>
   </si>
   <si>
-    <t>Cherry Line Production 7:00AM - 3:30PM</t>
+    <t>Presize 7:00AM - 3:30PM</t>
   </si>
   <si>
-    <t>Cherry Line Sorting 7:00AM - 3:30PM</t>
-  </si>
-  <si>
-    <t>Operations 7:00AM - 3:30PM</t>
-  </si>
-  <si>
-    <t>Cherry Line Production 4:00PM - 12:30AM</t>
-  </si>
-  <si>
-    <t>Cherry Line Sorting 4:00PM - 12:30AM</t>
+    <t>Presize 4:00PM - 12:30AM</t>
   </si>
 </sst>
 </file>
@@ -528,15 +519,15 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AS5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AK5" sqref="AK5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:18">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -548,52 +539,19 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="13"/>
-      <c r="AK2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10"/>
-      <c r="AQ2" s="10"/>
-      <c r="AR2" s="10"/>
-      <c r="AS2" s="13"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="13"/>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:18">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -603,44 +561,17 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="11"/>
-      <c r="AI3" s="11"/>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="11"/>
-      <c r="AM3" s="11"/>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="11"/>
-      <c r="AP3" s="11"/>
-      <c r="AQ3" s="11"/>
-      <c r="AR3" s="11"/>
-      <c r="AS3" s="14"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="14"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:18">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -652,50 +583,17 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL5" s="15"/>
-      <c r="AM5" s="15"/>
-      <c r="AN5" s="15"/>
-      <c r="AO5" s="15"/>
-      <c r="AP5" s="15"/>
-      <c r="AQ5" s="15"/>
-      <c r="AR5" s="15"/>
-      <c r="AS5" s="16"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -704,12 +602,6 @@
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="J2:R3"/>
     <mergeCell ref="J5:R5"/>
-    <mergeCell ref="S2:AA3"/>
-    <mergeCell ref="S5:AA5"/>
-    <mergeCell ref="AB2:AJ3"/>
-    <mergeCell ref="AB5:AJ5"/>
-    <mergeCell ref="AK2:AS3"/>
-    <mergeCell ref="AK5:AS5"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
saving while workspace crashes
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>Friday March 4, 2016</t>
   </si>
@@ -24,7 +24,10 @@
     <t>Presize 7:00AM - 3:30PM</t>
   </si>
   <si>
-    <t>Presize 4:00PM - 12:30AM</t>
+    <t>Line Operator</t>
+  </si>
+  <si>
+    <t>Alan Zanotto</t>
   </si>
 </sst>
 </file>
@@ -61,7 +64,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,12 +80,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3F7FBF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border/>
@@ -162,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="10">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -191,33 +188,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -519,15 +489,15 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:9">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -539,19 +509,8 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="13"/>
-    </row>
-    <row r="3" spans="1:18">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -561,17 +520,8 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="14"/>
-    </row>
-    <row r="5" spans="1:18">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -583,25 +533,376 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="16"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A2:I3"/>
     <mergeCell ref="A5:I5"/>
-    <mergeCell ref="J2:R3"/>
-    <mergeCell ref="J5:R5"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
print logic is implement, now just bug fixing it
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -16,18 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
-    <t>Friday March 4, 2016</t>
+    <t>Saturday March 5, 2016</t>
   </si>
   <si>
     <t>Presize 7:00AM - 3:30PM</t>
   </si>
   <si>
-    <t>Line Operator</t>
-  </si>
-  <si>
-    <t>Alan Zanotto</t>
+    <t>Presize 4:00PM - 12:30AM</t>
   </si>
 </sst>
 </file>
@@ -64,7 +61,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,6 +77,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3F7FBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border/>
@@ -159,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -188,6 +191,33 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -489,15 +519,15 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:18">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -509,8 +539,19 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="4"/>
+      <c r="J2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="13"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:18">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -520,8 +561,17 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="5"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="14"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:18">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -533,376 +583,25 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+      <c r="J5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>2</v>
-      </c>
-      <c r="G22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>2</v>
-      </c>
-      <c r="G25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>2</v>
-      </c>
-      <c r="G28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E34" t="s">
-        <v>2</v>
-      </c>
-      <c r="G34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>3</v>
-      </c>
-      <c r="G35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" t="s">
-        <v>2</v>
-      </c>
-      <c r="G37" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>2</v>
-      </c>
-      <c r="E40" t="s">
-        <v>2</v>
-      </c>
-      <c r="G40" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" t="s">
-        <v>3</v>
-      </c>
-      <c r="G41" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>2</v>
-      </c>
-      <c r="G43" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" t="s">
-        <v>3</v>
-      </c>
-      <c r="G44" t="s">
-        <v>3</v>
-      </c>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A2:I3"/>
     <mergeCell ref="A5:I5"/>
+    <mergeCell ref="J2:R3"/>
+    <mergeCell ref="J5:R5"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
logical errors corected.  schedule now prints peoples positions.  going to have to test this more
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -16,15 +16,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>Saturday March 5, 2016</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+  <si>
+    <t>Friday March 4, 2016</t>
   </si>
   <si>
     <t>Presize 7:00AM - 3:30PM</t>
   </si>
   <si>
-    <t>Presize 4:00PM - 12:30AM</t>
+    <t>Bin Filler</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Doris Reynolds</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zabada Mohammed</t>
+  </si>
+  <si>
+    <t>Forklift</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> George Dunn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Don Coles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> George C Brown</t>
+  </si>
+  <si>
+    <t>Line Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parveen Gopal</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isabel Roseen</t>
+  </si>
+  <si>
+    <t>Non Rotational</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elaine Roseen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Janeanne Reiswig</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sandra Martin</t>
   </si>
 </sst>
 </file>
@@ -61,7 +103,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,12 +119,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3F7FBF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border/>
@@ -162,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="10">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -191,33 +227,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -519,15 +528,15 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:9">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -539,19 +548,8 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="13"/>
-    </row>
-    <row r="3" spans="1:18">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -561,17 +559,8 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="14"/>
-    </row>
-    <row r="5" spans="1:18">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -583,25 +572,87 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="18" t="s">
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="16"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A2:I3"/>
     <mergeCell ref="A5:I5"/>
-    <mergeCell ref="J2:R3"/>
-    <mergeCell ref="J5:R5"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cleared array so it wouldnt remember old positions
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -16,57 +16,711 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
-  <si>
-    <t>Friday March 4, 2016</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="235">
+  <si>
+    <t>Friday March 18, 2016</t>
   </si>
   <si>
     <t>Presize 7:00AM - 3:30PM</t>
   </si>
   <si>
+    <t>A Line 7:00AM - 3:30PM</t>
+  </si>
+  <si>
+    <t>Cherry Line Production 7:00AM - 3:30PM</t>
+  </si>
+  <si>
+    <t>Cherry Line Sorting 7:00AM - 3:30PM</t>
+  </si>
+  <si>
     <t>Bin Filler</t>
   </si>
   <si>
+    <t>Line Operator</t>
+  </si>
+  <si>
+    <t>Sort - A5</t>
+  </si>
+  <si>
+    <t>BMO</t>
+  </si>
+  <si>
+    <t>Bliss Helper</t>
+  </si>
+  <si>
+    <t>Sort 1 (Non Rotational)</t>
+  </si>
+  <si>
+    <t>Mapping 9</t>
+  </si>
+  <si>
+    <t>Sort 17</t>
+  </si>
+  <si>
+    <t>Sort 25</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Doris Reynolds</t>
   </si>
   <si>
+    <t xml:space="preserve"> Lori Carter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gerald Kunz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dale  Driscoll</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barb Silvester</t>
+  </si>
+  <si>
+    <t>UNFILLED POSITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sukhdev Atwal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jean Charest</t>
+  </si>
+  <si>
+    <t>Balbir Kaila</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Zabada Mohammed</t>
   </si>
   <si>
+    <t xml:space="preserve"> Judy Matsalla</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brian High</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurbakhash Aujla</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paramjeet Gill</t>
+  </si>
+  <si>
+    <t>Katherine Morgan-Heyes</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>Sort - A6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Joyce Salga</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Davinder Lit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ipin Hu</t>
+  </si>
+  <si>
+    <t>Ibriam Stange</t>
+  </si>
+  <si>
     <t>Forklift</t>
   </si>
   <si>
+    <t xml:space="preserve"> Wendy Casorso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ron Engene</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shannon Fehr</t>
+  </si>
+  <si>
+    <t>Scanner / Stacker</t>
+  </si>
+  <si>
     <t xml:space="preserve"> George Dunn</t>
   </si>
   <si>
+    <t xml:space="preserve"> Kelsey Iceton</t>
+  </si>
+  <si>
+    <t>Sort 2</t>
+  </si>
+  <si>
+    <t>Sort 10</t>
+  </si>
+  <si>
+    <t>Sort 18</t>
+  </si>
+  <si>
+    <t>Sort 26</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Don Coles</t>
   </si>
   <si>
+    <t>Palletizer</t>
+  </si>
+  <si>
+    <t>Sort - A7</t>
+  </si>
+  <si>
+    <t>Stamping</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Debbie Szing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tirath Mann</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rajwinder Khun Khun</t>
+  </si>
+  <si>
+    <t>Anna-Lissa Raymond</t>
+  </si>
+  <si>
     <t xml:space="preserve"> George C Brown</t>
   </si>
   <si>
-    <t>Line Operator</t>
+    <t xml:space="preserve"> Javed Ali</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jerry Engene</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurdev  Kajla</t>
+  </si>
+  <si>
+    <t>Line Operator #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marcella Bartolomeoli</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jaswinder Purewal</t>
+  </si>
+  <si>
+    <t>Vidya Banga</t>
+  </si>
+  <si>
+    <t>Levol Williams</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Linda St. Amand</t>
+  </si>
+  <si>
+    <t>Bob Young</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Joginder Lalli</t>
+  </si>
+  <si>
+    <t>Judy Haworth</t>
+  </si>
+  <si>
+    <t>Zulekha Bawa</t>
+  </si>
+  <si>
+    <t>Labeller</t>
+  </si>
+  <si>
+    <t>Sort - A8</t>
+  </si>
+  <si>
+    <t>Dumper Operator</t>
   </si>
   <si>
     <t xml:space="preserve"> Parveen Gopal</t>
   </si>
   <si>
-    <t>QC</t>
+    <t xml:space="preserve"> Gail Johnson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurdev Bains</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alec Kovacs</t>
+  </si>
+  <si>
+    <t>Line Operator #2</t>
+  </si>
+  <si>
+    <t>Manifolds 3</t>
+  </si>
+  <si>
+    <t>Manifolds 11</t>
+  </si>
+  <si>
+    <t>Sort 19</t>
+  </si>
+  <si>
+    <t>Sort 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Julie Hackman</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cindy Stubbs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Balbir Mann</t>
+  </si>
+  <si>
+    <t>Sarabjeet Khera</t>
+  </si>
+  <si>
+    <t>James Fraser</t>
+  </si>
+  <si>
+    <t>Trays</t>
+  </si>
+  <si>
+    <t>Flow Control - A8</t>
+  </si>
+  <si>
+    <t>Stacker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Judy Ann Seymour</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Avtar Lit</t>
+  </si>
+  <si>
+    <t>Joachim Lenz</t>
+  </si>
+  <si>
+    <t>Kathy Hilstob</t>
   </si>
   <si>
     <t xml:space="preserve"> Isabel Roseen</t>
   </si>
   <si>
+    <t xml:space="preserve"> Ranjeet Deol</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fay Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Djibrilou Tall</t>
+  </si>
+  <si>
+    <t>Bliss #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Daryl Galigan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sukhwinder Nijjar</t>
+  </si>
+  <si>
+    <t>Kashmiri Bhatia</t>
+  </si>
+  <si>
+    <t>Dylan Anderson</t>
+  </si>
+  <si>
+    <t>Colton Gaudet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cheryl Deboer</t>
+  </si>
+  <si>
     <t>Non Rotational</t>
   </si>
   <si>
+    <t>Flow Control - A9</t>
+  </si>
+  <si>
+    <t>Kelsey Sacht</t>
+  </si>
+  <si>
+    <t>Sort 4</t>
+  </si>
+  <si>
+    <t>Sort 12</t>
+  </si>
+  <si>
+    <t>Sort 20</t>
+  </si>
+  <si>
+    <t>Sort 28</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Elaine Roseen</t>
   </si>
   <si>
+    <t xml:space="preserve"> Jane Wu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dora Strachan</t>
+  </si>
+  <si>
+    <t>Jesse Fred</t>
+  </si>
+  <si>
+    <t>Bliss #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chris Bauer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sarbjit Kohar</t>
+  </si>
+  <si>
+    <t>Jodi Buchinski</t>
+  </si>
+  <si>
+    <t>Amber Crittenden</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Janeanne Reiswig</t>
   </si>
   <si>
+    <t xml:space="preserve"> Kathy Jensen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sue Marks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ramandeep Toor</t>
+  </si>
+  <si>
+    <t>Sudesh Sarowa</t>
+  </si>
+  <si>
+    <t>Zack Dupont</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Sandra Martin</t>
+  </si>
+  <si>
+    <t>A Bliss</t>
+  </si>
+  <si>
+    <t>Flow Control - A10</t>
+  </si>
+  <si>
+    <t>Forklift (Loading)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ray Dixon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jesse Van Apeldoorn</t>
+  </si>
+  <si>
+    <t>Cindy McKee</t>
+  </si>
+  <si>
+    <t>Jane Recco</t>
+  </si>
+  <si>
+    <t>Pauline Palatin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ann Cloutier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jennifer  Knight</t>
+  </si>
+  <si>
+    <t>Self Sampler</t>
+  </si>
+  <si>
+    <t>Mapping 5</t>
+  </si>
+  <si>
+    <t>Manifolds 13</t>
+  </si>
+  <si>
+    <t>Sort 21</t>
+  </si>
+  <si>
+    <t>Sort 29</t>
+  </si>
+  <si>
+    <t>F/L Operator</t>
+  </si>
+  <si>
+    <t>Flow Control - A11</t>
+  </si>
+  <si>
+    <t>Forklift (Paper/Culls)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lindi Karmason</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurjit Bassi</t>
+  </si>
+  <si>
+    <t>Gaurav Verma</t>
+  </si>
+  <si>
+    <t>Tyson Devlin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juanita Windels</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nadine Boltz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jakob Schlegal</t>
+  </si>
+  <si>
+    <t>Cull Paper/Sorter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Catherine Knox</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ranjit Kohar</t>
+  </si>
+  <si>
+    <t>Theresa Reiswig</t>
+  </si>
+  <si>
+    <t>Steve Bifford</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rukhmani Reddy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parmjit Dhaliwal</t>
+  </si>
+  <si>
+    <t>Doug Weddell</t>
+  </si>
+  <si>
+    <t>Derek Richard</t>
+  </si>
+  <si>
+    <t>F/L Dumper (6:45am)</t>
+  </si>
+  <si>
+    <t>Fill - A12</t>
+  </si>
+  <si>
+    <t>Forklift (Warehouse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Margie Butcher</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Donnely</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bobby  Kovacs</t>
+  </si>
+  <si>
+    <t>Sort 6</t>
+  </si>
+  <si>
+    <t>Sort 14</t>
+  </si>
+  <si>
+    <t>Sort 22</t>
+  </si>
+  <si>
+    <t>Sort 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vickee Anderson</t>
+  </si>
+  <si>
+    <t>Jagir Judge</t>
+  </si>
+  <si>
+    <t>Debbie Segert</t>
+  </si>
+  <si>
+    <t>Shannon Lancaster</t>
+  </si>
+  <si>
+    <t>Sort - A1</t>
+  </si>
+  <si>
+    <t>Fill - A13</t>
+  </si>
+  <si>
+    <t>Lidder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mary-Ann Korthals</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Judy Moyles</t>
+  </si>
+  <si>
+    <t>Barb Fisher</t>
+  </si>
+  <si>
+    <t>Harjot Randhawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jean Strachan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ross Izod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sheri Bessette</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jasbir Isser</t>
+  </si>
+  <si>
+    <t>Mohan Madurai</t>
+  </si>
+  <si>
+    <t>Ravi Dhillon</t>
+  </si>
+  <si>
+    <t>Sort - A2</t>
+  </si>
+  <si>
+    <t>Fill - A14</t>
+  </si>
+  <si>
+    <t>Manifolds 7</t>
+  </si>
+  <si>
+    <t>Sort 15</t>
+  </si>
+  <si>
+    <t>Sort 23</t>
+  </si>
+  <si>
+    <t>Sort 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Janice Koyama</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Judy Skrove</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sylvia Friedrich</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Valerie Wheatley</t>
+  </si>
+  <si>
+    <t>Hardeep Lally</t>
+  </si>
+  <si>
+    <t>Kris  Hogg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Theresa Olson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Razia Ahmad</t>
+  </si>
+  <si>
+    <t>Satpal Hans</t>
+  </si>
+  <si>
+    <t>Michael Ferguson</t>
+  </si>
+  <si>
+    <t>Sort - A3</t>
+  </si>
+  <si>
+    <t>Fill - A15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Branden Dubrett</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jesse Bryden</t>
+  </si>
+  <si>
+    <t>Gill Daoust</t>
+  </si>
+  <si>
+    <t>R.J. Lukinuk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Jansen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tim Skrove</t>
+  </si>
+  <si>
+    <t>Dumper Helper/Stacker</t>
+  </si>
+  <si>
+    <t>David McPherson</t>
+  </si>
+  <si>
+    <t>Sort 8</t>
+  </si>
+  <si>
+    <t>Sort 16</t>
+  </si>
+  <si>
+    <t>Sort 24</t>
+  </si>
+  <si>
+    <t>Sort 32</t>
+  </si>
+  <si>
+    <t>Sort - A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jasbir Bhatti</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bhupinder Dhaliwal</t>
+  </si>
+  <si>
+    <t>Ravpal Randhawa</t>
+  </si>
+  <si>
+    <t>Akashdeep Bajwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ed Fehr</t>
+  </si>
+  <si>
+    <t>BMO Helper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gurmel Dhaliwal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rajwinder Kullar</t>
+  </si>
+  <si>
+    <t>Melinda Mascarenhas</t>
+  </si>
+  <si>
+    <t>Gurinder Bajwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Karen Lohse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Karmjit Nahal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fatoumata Barry</t>
+  </si>
+  <si>
+    <t>Brenda Carter</t>
+  </si>
+  <si>
+    <t>Brittany Berisoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rick Sehn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kathy Yates</t>
   </si>
 </sst>
 </file>
@@ -74,7 +728,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -99,6 +753,24 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -198,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -228,6 +900,12 @@
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,15 +1206,15 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:AJ47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="AH45" sqref="AH45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:36">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -548,8 +1226,41 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="4"/>
+    </row>
+    <row r="3" spans="1:36">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -559,8 +1270,35 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="5"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J3" s="3"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="5"/>
+    </row>
+    <row r="5" spans="1:36">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -572,80 +1310,843 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+      <c r="J5" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="7"/>
+    </row>
+    <row r="7" spans="1:36">
+      <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
+      <c r="J7" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
+      <c r="L7" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
+      <c r="S7" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
+      <c r="U7" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
+      <c r="AB7" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
+      <c r="AD7" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
+      <c r="AF7" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
+      <c r="AH7" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
+    <row r="8" spans="1:36">
+      <c r="A8" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
+      <c r="J8" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
+      <c r="L8" s="11" t="s">
         <v>16</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="U8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH8" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36">
+      <c r="A9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH9" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36">
+      <c r="J10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH10" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36">
+      <c r="A11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="U11" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36">
+      <c r="A12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH12" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36">
+      <c r="A13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH13" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="U14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH14" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36">
+      <c r="U15" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB15" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH15" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36">
+      <c r="A16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="S16" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36">
+      <c r="A17" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="S17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB17" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF17" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH17" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36">
+      <c r="U18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB18" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD18" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF18" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH18" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36">
+      <c r="A19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="S19" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB19" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD19" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF19" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH19" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36">
+      <c r="A20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB20" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD20" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF20" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH20" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36">
+      <c r="S21" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="U21" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36">
+      <c r="A22" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="S22" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB22" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD22" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF22" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH22" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36">
+      <c r="A23" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="S23" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="U23" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB23" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD23" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF23" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH23" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36">
+      <c r="A24" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="U24" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB24" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD24" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF24" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH24" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36">
+      <c r="A25" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="S25" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB25" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD25" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF25" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH25" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36">
+      <c r="J26" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S26" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="U26" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36">
+      <c r="U27" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB27" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD27" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF27" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="AH27" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36">
+      <c r="J28" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="S28" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB28" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD28" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="AF28" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH28" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36">
+      <c r="J29" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="S29" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="U29" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB29" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD29" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF29" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="AH29" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36">
+      <c r="U30" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB30" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD30" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF30" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH30" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36">
+      <c r="J31" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L31" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="S31" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36">
+      <c r="J32" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="L32" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="S32" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB32" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD32" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF32" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="AH32" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36">
+      <c r="AB33" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD33" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF33" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="AH33" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36">
+      <c r="J34" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="L34" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="S34" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB34" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD34" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF34" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="AH34" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36">
+      <c r="J35" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="L35" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="S35" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB35" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="AD35" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF35" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="AH35" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36">
+      <c r="S36" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36">
+      <c r="J37" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="S37" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB37" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD37" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF37" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH37" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36">
+      <c r="J38" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="L38" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="S38" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB38" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD38" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF38" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="AH38" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36">
+      <c r="S39" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB39" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="AD39" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF39" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="AH39" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36">
+      <c r="J40" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="L40" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB40" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD40" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF40" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="AH40" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36">
+      <c r="J41" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="L41" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="S41" s="10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36">
+      <c r="S42" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="AB42" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="AD42" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="AF42" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH42" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36">
+      <c r="J43" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB43" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD43" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="AF43" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH43" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36">
+      <c r="J44" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="S44" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB44" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD44" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="AF44" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH44" s="11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36">
+      <c r="S45" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB45" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AD45" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="AF45" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="AH45" s="11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36">
+      <c r="S46" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36">
+      <c r="S47" s="11" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -653,6 +2154,12 @@
   <mergeCells>
     <mergeCell ref="A2:I3"/>
     <mergeCell ref="A5:I5"/>
+    <mergeCell ref="J2:R3"/>
+    <mergeCell ref="J5:R5"/>
+    <mergeCell ref="S2:AA3"/>
+    <mergeCell ref="S5:AA5"/>
+    <mergeCell ref="AB2:AJ3"/>
+    <mergeCell ref="AB5:AJ5"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>